<commit_message>
ajout contacteur aux commandes
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Commandes.xlsx
+++ b/EL - Electrical/Autre/Commandes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E79AC7-383D-4A81-B9F6-6AE4F0AFCEA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCBE83C-8066-4A15-8886-0F0936FD4F78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS components" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="47">
   <si>
     <t>Système</t>
   </si>
@@ -163,13 +163,19 @@
   </si>
   <si>
     <t>Romain FERNAND   : &lt;r.fernand@texense.com&gt;</t>
+  </si>
+  <si>
+    <t>854-1966</t>
+  </si>
+  <si>
+    <t>Contacteur guillotine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +202,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -217,7 +230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -294,11 +307,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -319,9 +341,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -331,6 +350,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -614,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +663,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -664,7 +689,16 @@
       </c>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="F2">
         <f>1.2*E2</f>
         <v>0</v>
@@ -1030,7 +1064,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -1415,12 +1449,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="11" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1861,7 +1895,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -2255,7 +2289,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -2656,7 +2690,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -2685,7 +2719,7 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>35</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -2705,7 +2739,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -2725,7 +2759,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>37</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -2745,7 +2779,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>39</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -3078,7 +3112,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -3446,7 +3480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -3467,7 +3501,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">

</xml_diff>

<commit_message>
ajout elmp sensor et commande variohm
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Commandes.xlsx
+++ b/EL - Electrical/Autre/Commandes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECBC205-DD26-46B6-9BE8-6204545B5809}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48662CC1-1EBC-4817-955C-DC221C7FF211}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS components" sheetId="1" r:id="rId1"/>
@@ -181,12 +181,6 @@
     <t>Arduino Uno</t>
   </si>
   <si>
-    <t>PY2-C-25-P</t>
-  </si>
-  <si>
-    <t>Linear motion position sensor</t>
-  </si>
-  <si>
     <t>Pression huile moteur</t>
   </si>
   <si>
@@ -227,6 +221,12 @@
   </si>
   <si>
     <t>Connecteur méca</t>
+  </si>
+  <si>
+    <t>ELPM-25</t>
+  </si>
+  <si>
+    <t>Motorsport linear motion position sensor</t>
   </si>
 </sst>
 </file>
@@ -467,11 +467,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1766,7 +1766,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1810,22 +1810,22 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F2">
         <f>1.2*E2</f>
@@ -1848,13 +1848,13 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F24" si="0">1.2*E3</f>
@@ -1872,7 +1872,7 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1880,13 +1880,13 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1912,13 +1912,13 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
         <v>58</v>
-      </c>
-      <c r="C5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" t="s">
-        <v>60</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -1936,7 +1936,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1944,10 +1944,10 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -2252,11 +2252,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
       <c r="D1" s="11" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
carte afficheur rapport et commandes
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Commandes.xlsx
+++ b/EL - Electrical/Autre/Commandes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48662CC1-1EBC-4817-955C-DC221C7FF211}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8C3E8D-8B35-4E9E-BF41-25FF719D2973}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS components" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="77">
   <si>
     <t>Système</t>
   </si>
@@ -67,12 +67,6 @@
     <t>Télémétrie</t>
   </si>
   <si>
-    <t>Passage de vitesse</t>
-  </si>
-  <si>
-    <t>électronique</t>
-  </si>
-  <si>
     <t>S80 Spliced Loom Kit</t>
   </si>
   <si>
@@ -227,13 +221,83 @@
   </si>
   <si>
     <t>Motorsport linear motion position sensor</t>
+  </si>
+  <si>
+    <t>507-949</t>
+  </si>
+  <si>
+    <t>numéro de la commande</t>
+  </si>
+  <si>
+    <t>Boîtier IP66</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(10/102018)</t>
+    </r>
+  </si>
+  <si>
+    <t>pour arduino uno(voir place des souriau)</t>
+  </si>
+  <si>
+    <t>Carte avant</t>
+  </si>
+  <si>
+    <t>Carte arrière</t>
+  </si>
+  <si>
+    <t>Tableau de bord</t>
+  </si>
+  <si>
+    <t>124-5482</t>
+  </si>
+  <si>
+    <t>Ruban led</t>
+  </si>
+  <si>
+    <t>pour le compte tour ( 2x moins chère chez adafruit !)</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Ruban LED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,8 +331,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,8 +388,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF57171"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -414,11 +521,193 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -457,9 +746,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -473,12 +759,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF57171"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -753,582 +1114,665 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="15" t="s">
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="F2" s="32">
+        <v>1.022</v>
+      </c>
+      <c r="G2" s="32">
+        <f>1.2*F2</f>
+        <v>1.2263999999999999</v>
+      </c>
+      <c r="H2" s="33">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="32">
+        <v>5</v>
+      </c>
+      <c r="J2" s="34">
+        <f>I2*F2*(1-H2)</f>
+        <v>4.5990000000000002</v>
+      </c>
+      <c r="K2" s="35">
+        <f>J2*1.2</f>
+        <v>5.5187999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="49"/>
+      <c r="B3" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D3" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="17">
-        <v>1.022</v>
-      </c>
-      <c r="F2" s="17">
-        <f>1.2*E2</f>
-        <v>1.2263999999999999</v>
-      </c>
-      <c r="G2" s="18">
+      <c r="E3" s="39"/>
+      <c r="F3" s="39">
+        <v>20.57</v>
+      </c>
+      <c r="G3" s="39">
+        <f t="shared" ref="G3:G25" si="0">1.2*F3</f>
+        <v>24.684000000000001</v>
+      </c>
+      <c r="H3" s="40">
         <v>0.1</v>
       </c>
-      <c r="H2" s="17">
-        <v>5</v>
-      </c>
-      <c r="I2" s="19">
-        <f>H2*E2*(1-G2)</f>
-        <v>4.5990000000000002</v>
-      </c>
-      <c r="J2" s="19">
-        <f>I2*1.2</f>
-        <v>5.5187999999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12">
-        <v>20.57</v>
-      </c>
-      <c r="F3" s="12">
-        <f t="shared" ref="F3:F24" si="0">1.2*E3</f>
-        <v>24.684000000000001</v>
-      </c>
-      <c r="G3" s="13">
+      <c r="I3" s="39">
+        <v>2</v>
+      </c>
+      <c r="J3" s="41">
+        <f t="shared" ref="J3:J21" si="1">I3*F3*(1-H3)</f>
+        <v>37.026000000000003</v>
+      </c>
+      <c r="K3" s="42">
+        <f>J3*1.2</f>
+        <v>44.431200000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="50"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="47">
+        <f>SUM(F2:F3)</f>
+        <v>21.591999999999999</v>
+      </c>
+      <c r="G4" s="47">
+        <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
+        <v>25.910400000000003</v>
+      </c>
+      <c r="H4" s="47">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="I4" s="47">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J4" s="47">
+        <f t="shared" si="2"/>
+        <v>41.625</v>
+      </c>
+      <c r="K4" s="47">
+        <f t="shared" si="2"/>
+        <v>49.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="51">
+        <v>2</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="16">
+        <v>13.59</v>
+      </c>
+      <c r="G5" s="16">
+        <f t="shared" si="0"/>
+        <v>16.308</v>
+      </c>
+      <c r="H5" s="17">
         <v>0.1</v>
       </c>
-      <c r="H3" s="12">
+      <c r="I5" s="16">
         <v>2</v>
       </c>
-      <c r="I3" s="20">
-        <f t="shared" ref="I3:I20" si="1">H3*E3*(1-G3)</f>
-        <v>37.026000000000003</v>
-      </c>
-      <c r="J3" s="20">
-        <f t="shared" ref="J3:J24" si="2">I3*1.2</f>
-        <v>44.431200000000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G4" s="13">
+      <c r="J5" s="18">
+        <f t="shared" si="1"/>
+        <v>24.462</v>
+      </c>
+      <c r="K5" s="18">
+        <f t="shared" ref="K3:K25" si="3">J5*1.2</f>
+        <v>29.354399999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="51"/>
+      <c r="B6" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="13">
         <v>0.1</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J4" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="13">
+      <c r="I6" s="12"/>
+      <c r="J6" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="51"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="17">
         <v>0.1</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J6" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="51"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
-      <c r="F8" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="13">
+      <c r="F8" s="12"/>
+      <c r="G8" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="13">
         <v>0.1</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="51"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
-      <c r="F9" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="13">
+      <c r="F9" s="12"/>
+      <c r="G9" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="13">
         <v>0.1</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="51"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
-      <c r="F10" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="13">
+      <c r="F10" s="12"/>
+      <c r="G10" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="13">
         <v>0.1</v>
       </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="51"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="13">
+      <c r="F11" s="12"/>
+      <c r="G11" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="13">
         <v>0.1</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="51"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="13">
+      <c r="F12" s="12"/>
+      <c r="G12" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="13">
         <v>0.1</v>
       </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="51"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
-      <c r="F13" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="13">
+      <c r="F13" s="12"/>
+      <c r="G13" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="13">
         <v>0.1</v>
       </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="51"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="13">
+      <c r="F14" s="12"/>
+      <c r="G14" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
         <v>0.1</v>
       </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="29"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
-      <c r="F15" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="13">
+      <c r="F15" s="12"/>
+      <c r="G15" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="13">
         <v>0.1</v>
       </c>
-      <c r="H15" s="12"/>
-      <c r="I15" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="29"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
-      <c r="F16" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="13">
+      <c r="F16" s="12"/>
+      <c r="G16" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="13">
         <v>0.1</v>
       </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="29"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
-      <c r="F17" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="13">
+      <c r="F17" s="12"/>
+      <c r="G17" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="13">
         <v>0.1</v>
       </c>
-      <c r="H17" s="12"/>
-      <c r="I17" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="29"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="13">
+      <c r="F18" s="12"/>
+      <c r="G18" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="13">
         <v>0.1</v>
       </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="29"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
-      <c r="F19" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="13">
+      <c r="F19" s="12"/>
+      <c r="G19" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="13">
         <v>0.1</v>
       </c>
-      <c r="H19" s="12"/>
-      <c r="I19" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="29"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
-      <c r="F20" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <f t="shared" ref="I21:I24" si="3">H21*E21</f>
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I22">
+      <c r="F20" s="12"/>
+      <c r="G20" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="I20" s="12"/>
+      <c r="J20" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="29"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="J22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I23">
+        <f t="shared" ref="J22:J25" si="4">I22*F22</f>
+        <v>0</v>
+      </c>
+      <c r="K22">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="J23">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K23">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="J24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A5:A14"/>
+    <mergeCell ref="A2:A4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
-            <xm:f>Données!$A$1:$A$4</xm:f>
+            <xm:f>Données!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A21</xm:sqref>
+          <xm:sqref>B22</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F15CAACE-BD3C-4F3F-8AD7-94DA2B82CEF2}">
+          <x14:formula1>
+            <xm:f>Données!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B21</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1338,13 +1782,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1358,12 +1805,17 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1376,7 +1828,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,7 +1874,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="29"/>
       <c r="F2">
         <f>1.2*E2</f>
         <v>0</v>
@@ -1436,7 +1889,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="29"/>
       <c r="F3">
         <f t="shared" ref="F3:F24" si="0">1.2*E3</f>
         <v>0</v>
@@ -1450,7 +1904,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29"/>
       <c r="F4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1464,7 +1919,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="29"/>
       <c r="F5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1478,7 +1934,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="29"/>
       <c r="F6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1492,7 +1949,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29"/>
       <c r="F7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1506,7 +1964,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="29"/>
       <c r="F8">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1520,7 +1979,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="29"/>
       <c r="F9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1534,7 +1994,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="29"/>
       <c r="F10">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1548,7 +2009,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="29"/>
       <c r="F11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1562,7 +2024,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29"/>
       <c r="F12">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1576,7 +2039,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="29"/>
       <c r="F13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1590,7 +2054,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29"/>
       <c r="F14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1604,7 +2069,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="29"/>
       <c r="F15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1618,7 +2084,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="29"/>
       <c r="F16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1632,7 +2099,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="29"/>
       <c r="F17">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1646,7 +2114,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="29"/>
       <c r="F18">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1660,7 +2129,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="29"/>
       <c r="F19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1674,7 +2144,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="29"/>
       <c r="F20">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1688,7 +2159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F21">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1702,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F22">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1716,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F23">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1730,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1748,12 +2219,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
-            <xm:f>Données!$A$1:$A$4</xm:f>
+            <xm:f>Données!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A21</xm:sqref>
+          <xm:sqref>A21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{74EB11D5-595D-4F81-BCDC-E78475ACEDAA}">
+          <x14:formula1>
+            <xm:f>Données!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1765,8 +2242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2975CF6-F759-4AB5-BD70-F4541FA768DC}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1810,22 +2287,22 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>65</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F2">
         <f>1.2*E2</f>
@@ -1843,18 +2320,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F24" si="0">1.2*E3</f>
@@ -1872,21 +2349,21 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
@@ -1904,21 +2381,21 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
         <v>56</v>
-      </c>
-      <c r="C5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>58</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -1936,18 +2413,16 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="29"/>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -1962,7 +2437,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29"/>
       <c r="F7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1976,7 +2452,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="29"/>
       <c r="F8">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1990,7 +2467,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="29"/>
       <c r="F9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2004,7 +2482,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="29"/>
       <c r="F10">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2018,7 +2497,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="29"/>
       <c r="F11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2032,7 +2512,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29"/>
       <c r="F12">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2046,7 +2527,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="29"/>
       <c r="F13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2060,7 +2542,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29"/>
       <c r="F14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2074,7 +2557,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="29"/>
       <c r="F15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2088,7 +2572,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="29"/>
       <c r="F16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2102,7 +2587,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="29"/>
       <c r="F17">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2116,7 +2602,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="29"/>
       <c r="F18">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2130,7 +2617,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="29"/>
       <c r="F19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2144,7 +2632,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="29"/>
       <c r="F20">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2158,7 +2647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F21">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2172,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F22">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2186,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F23">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2200,7 +2689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2218,12 +2707,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4380C4A4-E62E-475A-A73D-70090E7E2E9A}">
           <x14:formula1>
-            <xm:f>Données!$A$1:$A$4</xm:f>
+            <xm:f>Données!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A21</xm:sqref>
+          <xm:sqref>A21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5B58D1E6-4568-4AB6-9373-5555FB956C9D}">
+          <x14:formula1>
+            <xm:f>Données!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2236,7 +2731,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2252,13 +2747,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="A1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
       <c r="D1" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2298,13 +2793,13 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
       </c>
       <c r="E3">
         <v>81</v>
@@ -2327,13 +2822,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="E4">
         <v>110</v>
@@ -2353,13 +2848,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
         <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -2664,7 +3159,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
-            <xm:f>Données!$A$1:$A$4</xm:f>
+            <xm:f>Données!$A$1:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A22</xm:sqref>
         </x14:dataValidation>
@@ -2678,8 +3173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:J24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2728,7 +3223,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2">
         <f>1.2*E2</f>
@@ -3058,7 +3553,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
-            <xm:f>Données!$A$1:$A$4</xm:f>
+            <xm:f>Données!$A$1:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A21</xm:sqref>
         </x14:dataValidation>
@@ -3073,7 +3568,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3092,7 +3587,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -3122,10 +3617,10 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2">
         <f>1.2*E2</f>
@@ -3145,10 +3640,10 @@
         <v>10</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F23" si="0">1.2*E3</f>
@@ -3168,10 +3663,10 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
@@ -3459,7 +3954,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
-            <xm:f>Données!$A$1:$A$4</xm:f>
+            <xm:f>Données!$A$1:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A20</xm:sqref>
         </x14:dataValidation>
@@ -3474,7 +3969,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3518,15 +4013,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
+    <row r="2" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
+        <v>70</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <f>1.2*E2</f>
@@ -3541,12 +4036,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
+        <v>70</v>
+      </c>
       <c r="C3" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F24" si="0">1.2*E3</f>
@@ -3561,52 +4059,61 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>70</v>
+      </c>
       <c r="C4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C5" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="D5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
         <v>29</v>
       </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
       <c r="D6" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -3621,7 +4128,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29"/>
       <c r="F7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3635,7 +4143,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="29"/>
       <c r="F8">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3649,7 +4158,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="29"/>
       <c r="F9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3663,7 +4173,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="29"/>
       <c r="F10">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3677,7 +4188,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="29"/>
       <c r="F11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3691,7 +4203,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29"/>
       <c r="F12">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3705,7 +4218,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="29"/>
       <c r="F13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3719,7 +4233,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29"/>
       <c r="F14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3733,7 +4248,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="29"/>
       <c r="F15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3747,7 +4263,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="29"/>
       <c r="F16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3761,7 +4278,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="29"/>
       <c r="F17">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3775,7 +4293,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="29"/>
       <c r="F18">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3789,7 +4308,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="29"/>
       <c r="F19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3803,7 +4323,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="29"/>
       <c r="F20">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3817,7 +4338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F21">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3831,7 +4352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F22">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3845,7 +4366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F23">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3859,7 +4380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3878,12 +4399,18 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
           <x14:formula1>
-            <xm:f>Données!$A$1:$A$4</xm:f>
+            <xm:f>Données!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A21</xm:sqref>
+          <xm:sqref>A21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{523A28AA-3BA2-47B7-8A1A-0DE4382AF599}">
+          <x14:formula1>
+            <xm:f>Données!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3896,7 +4423,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3941,6 +4468,9 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
       <c r="F2">
         <f>1.2*E2</f>
         <v>0</v>
@@ -3955,6 +4485,9 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
       <c r="F3">
         <f t="shared" ref="F3:F24" si="0">1.2*E3</f>
         <v>0</v>
@@ -3969,6 +4502,9 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
       <c r="F4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3983,6 +4519,9 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
       <c r="F5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3997,6 +4536,9 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
       <c r="F6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4011,6 +4553,9 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
       <c r="F7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4025,6 +4570,9 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
       <c r="F8">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4039,6 +4587,9 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
       <c r="F9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4053,6 +4604,9 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
       <c r="F10">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4067,6 +4621,9 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
       <c r="F11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4269,7 +4826,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000000000000}">
           <x14:formula1>
-            <xm:f>Données!$A$1:$A$4</xm:f>
+            <xm:f>Données!$A$1:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A21</xm:sqref>
         </x14:dataValidation>
@@ -4331,13 +4888,13 @@
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F2">
         <f>1.2*E2</f>
@@ -4418,7 +4975,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{83A983CF-8CAD-41B1-865B-95D300006522}">
           <x14:formula1>
-            <xm:f>Données!$A$1:$A$4</xm:f>
+            <xm:f>Données!$A$1:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A6</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
modif commande et connecteurs
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Commandes.xlsx
+++ b/EL - Electrical/Autre/Commandes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AC5880-D61B-48BD-91AA-201C65E9AD44}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45A824E-8630-482B-AC84-AB4DD532CEBD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS components" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="99">
   <si>
     <t>Système</t>
   </si>
@@ -306,45 +306,6 @@
   </si>
   <si>
     <t>BSPD</t>
-  </si>
-  <si>
-    <t>221-5535</t>
-  </si>
-  <si>
-    <t>NE555</t>
-  </si>
-  <si>
-    <t>timer BSPD</t>
-  </si>
-  <si>
-    <t>305-181</t>
-  </si>
-  <si>
-    <t>porte NOR</t>
-  </si>
-  <si>
-    <t>quadruple</t>
-  </si>
-  <si>
-    <t>463-870</t>
-  </si>
-  <si>
-    <t>Comparateur 2 entrées</t>
-  </si>
-  <si>
-    <t>par paquet de 50</t>
-  </si>
-  <si>
-    <t>par paquet de 20</t>
-  </si>
-  <si>
-    <t>541-9566</t>
-  </si>
-  <si>
-    <t>Double bascule flip-flop</t>
-  </si>
-  <si>
-    <t>par paquet de 5</t>
   </si>
   <si>
     <t>1012 £</t>
@@ -981,15 +942,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1003,8 +955,17 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1293,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,8 +1309,8 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
-        <v>110</v>
+      <c r="A2" s="61" t="s">
+        <v>97</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>67</v>
@@ -1386,7 +1347,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
+      <c r="A3" s="62"/>
       <c r="B3" s="40" t="s">
         <v>65</v>
       </c>
@@ -1420,7 +1381,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="57"/>
+      <c r="A4" s="62"/>
       <c r="B4" s="42"/>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -1453,8 +1414,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="64" t="s">
-        <v>111</v>
+      <c r="A5" s="63" t="s">
+        <v>98</v>
       </c>
       <c r="B5" s="43" t="s">
         <v>67</v>
@@ -1491,7 +1452,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="64"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="42"/>
       <c r="C6" s="33"/>
       <c r="D6" s="33"/>
@@ -1507,15 +1468,15 @@
         <v>43.46</v>
       </c>
       <c r="L6" s="55" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="63"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="57" t="s">
         <v>72</v>
       </c>
       <c r="D7" s="34" t="s">
@@ -1547,7 +1508,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="63"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="40" t="s">
         <v>10</v>
       </c>
@@ -1583,7 +1544,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="63"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="40" t="s">
         <v>10</v>
       </c>
@@ -1619,11 +1580,11 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="63"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="58" t="s">
         <v>78</v>
       </c>
       <c r="D10" s="14" t="s">
@@ -1655,151 +1616,98 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="63"/>
-      <c r="B11" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="C11" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="F11" s="11">
-        <v>0.29899999999999999</v>
-      </c>
+      <c r="A11" s="60"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
       <c r="G11" s="11">
-        <f t="shared" si="0"/>
-        <v>0.35879999999999995</v>
+        <f t="shared" ref="G11:G14" si="4">1.2*F11</f>
+        <v>0</v>
       </c>
       <c r="H11" s="12">
         <v>0.1</v>
       </c>
-      <c r="I11" s="11">
-        <v>50</v>
-      </c>
+      <c r="I11" s="11"/>
       <c r="J11" s="17">
-        <f t="shared" si="1"/>
-        <v>13.455</v>
+        <f t="shared" ref="J11:J14" si="5">I11*F11*(1-H11)</f>
+        <v>0</v>
       </c>
       <c r="K11" s="17">
-        <f t="shared" si="3"/>
-        <v>16.146000000000001</v>
-      </c>
-      <c r="L11" t="s">
-        <v>100</v>
+        <f t="shared" ref="K11:K14" si="6">J11*1.2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="63"/>
-      <c r="B12" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" s="60" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F12" s="11">
-        <v>1.34</v>
-      </c>
+      <c r="A12" s="60"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
       <c r="G12" s="11">
-        <f t="shared" si="0"/>
-        <v>1.6080000000000001</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="H12" s="12">
         <v>0.1</v>
       </c>
-      <c r="I12" s="11">
-        <v>4</v>
-      </c>
+      <c r="I12" s="11"/>
       <c r="J12" s="17">
-        <f t="shared" si="1"/>
-        <v>4.8240000000000007</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="K12" s="17">
-        <f t="shared" si="3"/>
-        <v>5.7888000000000011</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="63"/>
-      <c r="B13" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="60" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>99</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="60"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="11">
-        <v>0.376</v>
-      </c>
+      <c r="F13" s="11"/>
       <c r="G13" s="11">
-        <f t="shared" si="0"/>
-        <v>0.45119999999999999</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="H13" s="12">
         <v>0.1</v>
       </c>
-      <c r="I13" s="11">
-        <v>20</v>
-      </c>
+      <c r="I13" s="11"/>
       <c r="J13" s="17">
-        <f t="shared" si="1"/>
-        <v>6.7679999999999998</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="K13" s="17">
-        <f t="shared" si="3"/>
-        <v>8.121599999999999</v>
-      </c>
-      <c r="L13" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>103</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="56"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="11"/>
-      <c r="F14" s="11">
-        <v>0.76800000000000002</v>
-      </c>
+      <c r="F14" s="11"/>
       <c r="G14" s="11">
-        <f t="shared" si="0"/>
-        <v>0.92159999999999997</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="H14" s="12">
         <v>0.1</v>
       </c>
-      <c r="I14" s="11">
-        <v>5</v>
-      </c>
+      <c r="I14" s="11"/>
       <c r="J14" s="17">
-        <f t="shared" si="1"/>
-        <v>3.456</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="K14" s="17">
-        <f t="shared" si="3"/>
-        <v>4.1471999999999998</v>
-      </c>
-      <c r="L14" t="s">
-        <v>104</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1944,7 +1852,7 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <f t="shared" ref="J21:J24" si="4">I21*F21</f>
+        <f t="shared" ref="J21:J24" si="7">I21*F21</f>
         <v>0</v>
       </c>
       <c r="K21">
@@ -1958,7 +1866,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K22">
@@ -1972,7 +1880,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K23">
@@ -1986,7 +1894,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K24">
@@ -2181,7 +2089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -2277,10 +2185,10 @@
         <v>65</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="F2">
         <f>1.2*E2</f>
@@ -2307,7 +2215,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="45">
-        <f t="shared" ref="F3:J3" si="0">SUM(F1:F2)</f>
+        <f t="shared" ref="F3:I3" si="0">SUM(F1:F2)</f>
         <v>0</v>
       </c>
       <c r="G3" s="45">
@@ -2322,11 +2230,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J3" s="62">
+      <c r="J3" s="59">
         <v>35.22</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -3270,11 +3178,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
       <c r="D1" s="10" t="s">
         <v>42</v>
       </c>
@@ -4256,7 +4164,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="45">
-        <f t="shared" ref="F5:J5" si="3">SUM(F3:F4)</f>
+        <f t="shared" ref="F5:I5" si="3">SUM(F3:F4)</f>
         <v>0</v>
       </c>
       <c r="G5" s="45">
@@ -4272,7 +4180,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="45" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
mAj du shield avant
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Commandes.xlsx
+++ b/EL - Electrical/Autre/Commandes.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45A824E-8630-482B-AC84-AB4DD532CEBD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E6B459-680E-4624-A511-073F1FE3CCC3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS components" sheetId="1" r:id="rId1"/>
     <sheet name="Watterott" sheetId="11" r:id="rId2"/>
     <sheet name="Mouser" sheetId="3" r:id="rId3"/>
-    <sheet name="Variohm" sheetId="10" r:id="rId4"/>
-    <sheet name="Texense" sheetId="4" r:id="rId5"/>
+    <sheet name="Texense" sheetId="4" r:id="rId4"/>
+    <sheet name="Variohm" sheetId="10" r:id="rId5"/>
     <sheet name="oscaro" sheetId="5" r:id="rId6"/>
     <sheet name="DTA Fast" sheetId="6" r:id="rId7"/>
     <sheet name="DUNKERMOTOREN" sheetId="7" r:id="rId8"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="113">
   <si>
     <t>Système</t>
   </si>
@@ -371,6 +371,48 @@
       <t>(10/11/2018)</t>
     </r>
   </si>
+  <si>
+    <t>12v to 5v 3A pour alim tdb</t>
+  </si>
+  <si>
+    <t>495-THN15-2411WIR</t>
+  </si>
+  <si>
+    <t>THN15 traco power</t>
+  </si>
+  <si>
+    <t>799-0228</t>
+  </si>
+  <si>
+    <t>mcp2562</t>
+  </si>
+  <si>
+    <t>can transceiver</t>
+  </si>
+  <si>
+    <t>lot de 10</t>
+  </si>
+  <si>
+    <t>628-3548</t>
+  </si>
+  <si>
+    <t>mcp2515</t>
+  </si>
+  <si>
+    <t>can controler</t>
+  </si>
+  <si>
+    <t>547-6294</t>
+  </si>
+  <si>
+    <t>quartz 16 MHz</t>
+  </si>
+  <si>
+    <t>quartz pour le can</t>
+  </si>
+  <si>
+    <t>lot de 5</t>
+  </si>
 </sst>
 </file>
 
@@ -379,7 +421,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,6 +504,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -948,13 +996,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="8" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1254,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,7 +1518,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="60"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="46" t="s">
         <v>10</v>
       </c>
@@ -1508,7 +1554,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="60"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="40" t="s">
         <v>10</v>
       </c>
@@ -1544,7 +1590,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="60"/>
+      <c r="A9" s="59"/>
       <c r="B9" s="40" t="s">
         <v>10</v>
       </c>
@@ -1580,11 +1626,11 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="60"/>
-      <c r="B10" s="13" t="s">
+      <c r="A10" s="59"/>
+      <c r="B10" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="57" t="s">
         <v>78</v>
       </c>
       <c r="D10" s="14" t="s">
@@ -1604,47 +1650,70 @@
         <v>0.1</v>
       </c>
       <c r="I10" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J10" s="16">
         <f>I10*F10*(1-H10)</f>
-        <v>24.462</v>
+        <v>12.231</v>
       </c>
       <c r="K10" s="16">
         <f>J10*1.2</f>
-        <v>29.354399999999998</v>
+        <v>14.677199999999999</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="60"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0.78900000000000003</v>
+      </c>
       <c r="G11" s="11">
         <f t="shared" ref="G11:G14" si="4">1.2*F11</f>
-        <v>0</v>
+        <v>0.94679999999999997</v>
       </c>
       <c r="H11" s="12">
         <v>0.1</v>
       </c>
-      <c r="I11" s="11"/>
+      <c r="I11" s="11">
+        <v>10</v>
+      </c>
       <c r="J11" s="17">
         <f t="shared" ref="J11:J14" si="5">I11*F11*(1-H11)</f>
-        <v>0</v>
+        <v>7.1010000000000009</v>
       </c>
       <c r="K11" s="17">
         <f t="shared" ref="K11:K14" si="6">J11*1.2</f>
-        <v>0</v>
+        <v>8.5212000000000003</v>
+      </c>
+      <c r="L11" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="60"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="F12" s="11"/>
       <c r="G12" s="11">
         <f t="shared" si="4"/>
@@ -1663,28 +1732,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="60"/>
-      <c r="B13" s="56"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+    <row r="13" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="59"/>
+      <c r="B13" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0.27600000000000002</v>
+      </c>
       <c r="G13" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.33119999999999999</v>
       </c>
       <c r="H13" s="12">
         <v>0.1</v>
       </c>
-      <c r="I13" s="11"/>
+      <c r="I13" s="11">
+        <v>5</v>
+      </c>
       <c r="J13" s="17">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.2420000000000002</v>
       </c>
       <c r="K13" s="17">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.4904000000000002</v>
+      </c>
+      <c r="L13" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2230,7 +2314,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J3" s="59">
+      <c r="J3" s="58">
         <v>35.22</v>
       </c>
       <c r="K3" s="7" t="s">
@@ -2258,15 +2342,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
     <col min="7" max="7" width="18.140625" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
@@ -2305,19 +2389,36 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
+    <row r="2" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2">
+        <v>54.72</v>
+      </c>
       <c r="F2">
         <f>1.2*E2</f>
-        <v>0</v>
+        <v>65.664000000000001</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
       </c>
       <c r="I2">
         <f>H2*E2</f>
-        <v>0</v>
+        <v>54.72</v>
       </c>
       <c r="J2">
         <f>I2*1.2</f>
-        <v>0</v>
+        <v>65.664000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2648,6 +2749,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -2670,499 +2772,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2975CF6-F759-4AB5-BD70-F4541FA768DC}">
-  <dimension ref="A1:K24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2">
-        <f>1.2*E2</f>
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <f>H2*E2</f>
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <f>I2*1.2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F24" si="0">1.2*E3</f>
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I24" si="1">H3*E3</f>
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J24" si="2">I3*1.2</f>
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
-      <c r="C6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26"/>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26"/>
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4380C4A4-E62E-475A-A73D-70090E7E2E9A}">
-          <x14:formula1>
-            <xm:f>Données!$A$1:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>A21</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5B58D1E6-4568-4AB6-9373-5555FB956C9D}">
-          <x14:formula1>
-            <xm:f>Données!$A$1:$A$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2:A20</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3626,6 +3240,494 @@
             <xm:f>Données!$A$1:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A22</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2975CF6-F759-4AB5-BD70-F4541FA768DC}">
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2">
+        <f>1.2*E2</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <f>H2*E2</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>I2*1.2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F24" si="0">1.2*E3</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I24" si="1">H3*E3</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J24" si="2">I3*1.2</f>
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="26"/>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="26"/>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26"/>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="26"/>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="26"/>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="26"/>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="26"/>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="26"/>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="26"/>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="26"/>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="26"/>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="26"/>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="26"/>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4380C4A4-E62E-475A-A73D-70090E7E2E9A}">
+          <x14:formula1>
+            <xm:f>Données!$A$1:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>A21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5B58D1E6-4568-4AB6-9373-5555FB956C9D}">
+          <x14:formula1>
+            <xm:f>Données!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Ajout commande palette, composant carte avant et afficheur Tdb
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Commandes.xlsx
+++ b/EL - Electrical/Autre/Commandes.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E6B459-680E-4624-A511-073F1FE3CCC3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2460DC62-660F-4E07-B90E-28B8B7821895}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS components" sheetId="1" r:id="rId1"/>
     <sheet name="Watterott" sheetId="11" r:id="rId2"/>
     <sheet name="Mouser" sheetId="3" r:id="rId3"/>
-    <sheet name="Texense" sheetId="4" r:id="rId4"/>
-    <sheet name="Variohm" sheetId="10" r:id="rId5"/>
+    <sheet name="KazTechnologie" sheetId="12" r:id="rId4"/>
+    <sheet name="Texense" sheetId="4" r:id="rId5"/>
     <sheet name="oscaro" sheetId="5" r:id="rId6"/>
     <sheet name="DTA Fast" sheetId="6" r:id="rId7"/>
     <sheet name="DUNKERMOTOREN" sheetId="7" r:id="rId8"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="139">
   <si>
     <t>Système</t>
   </si>
@@ -174,54 +174,6 @@
   </si>
   <si>
     <t>Arduino Uno</t>
-  </si>
-  <si>
-    <t>Pression huile moteur</t>
-  </si>
-  <si>
-    <t>Pressur sensor</t>
-  </si>
-  <si>
-    <t>Position guillotine</t>
-  </si>
-  <si>
-    <t>EPT1200-K-16000-B-5-A</t>
-  </si>
-  <si>
-    <t>Pression frein</t>
-  </si>
-  <si>
-    <t>EPT3100-H-25000-A-5-A</t>
-  </si>
-  <si>
-    <t>EURO-WS-M10</t>
-  </si>
-  <si>
-    <t>Wheel speed sensor</t>
-  </si>
-  <si>
-    <t>Vitesse des roues</t>
-  </si>
-  <si>
-    <t>Pression essence</t>
-  </si>
-  <si>
-    <t>Dash 3</t>
-  </si>
-  <si>
-    <t>M8</t>
-  </si>
-  <si>
-    <t>M10</t>
-  </si>
-  <si>
-    <t>Connecteur méca</t>
-  </si>
-  <si>
-    <t>ELPM-25</t>
-  </si>
-  <si>
-    <t>Motorsport linear motion position sensor</t>
   </si>
   <si>
     <t>numéro de la commande</t>
@@ -372,18 +324,6 @@
     </r>
   </si>
   <si>
-    <t>12v to 5v 3A pour alim tdb</t>
-  </si>
-  <si>
-    <t>495-THN15-2411WIR</t>
-  </si>
-  <si>
-    <t>THN15 traco power</t>
-  </si>
-  <si>
-    <t>799-0228</t>
-  </si>
-  <si>
     <t>mcp2562</t>
   </si>
   <si>
@@ -393,9 +333,6 @@
     <t>lot de 10</t>
   </si>
   <si>
-    <t>628-3548</t>
-  </si>
-  <si>
     <t>mcp2515</t>
   </si>
   <si>
@@ -412,6 +349,147 @@
   </si>
   <si>
     <t>lot de 5</t>
+  </si>
+  <si>
+    <t>679-5596</t>
+  </si>
+  <si>
+    <t>467-598</t>
+  </si>
+  <si>
+    <t>cosse à sertir série 4809</t>
+  </si>
+  <si>
+    <t>pour KK 254</t>
+  </si>
+  <si>
+    <t>Connecteur 4 voie KK 254</t>
+  </si>
+  <si>
+    <t>mâle</t>
+  </si>
+  <si>
+    <t>467-611</t>
+  </si>
+  <si>
+    <t>femelle</t>
+  </si>
+  <si>
+    <t>10 unités</t>
+  </si>
+  <si>
+    <t>1 kit de 10</t>
+  </si>
+  <si>
+    <t>Afficheur 3 digit</t>
+  </si>
+  <si>
+    <t>863-4967</t>
+  </si>
+  <si>
+    <t>BA56-12SYKWA</t>
+  </si>
+  <si>
+    <t>877-0965</t>
+  </si>
+  <si>
+    <t>SA10-21SYKWA</t>
+  </si>
+  <si>
+    <t>Afficheur 1 digit</t>
+  </si>
+  <si>
+    <t>Paquet de 13</t>
+  </si>
+  <si>
+    <t>Paquet de 4</t>
+  </si>
+  <si>
+    <t>628-3532</t>
+  </si>
+  <si>
+    <t>799-0225</t>
+  </si>
+  <si>
+    <t>on en prends 5 au cas ou</t>
+  </si>
+  <si>
+    <t>734-6823</t>
+  </si>
+  <si>
+    <t>Bouton poussoir</t>
+  </si>
+  <si>
+    <t>173-2916</t>
+  </si>
+  <si>
+    <t>173-2922</t>
+  </si>
+  <si>
+    <t>173-2972</t>
+  </si>
+  <si>
+    <t>Connecteur 2 voie</t>
+  </si>
+  <si>
+    <t>Connecteur 3 voie</t>
+  </si>
+  <si>
+    <t>mâle KK254</t>
+  </si>
+  <si>
+    <t>Paquet de 5</t>
+  </si>
+  <si>
+    <t>296-4934</t>
+  </si>
+  <si>
+    <t>femelle KK254</t>
+  </si>
+  <si>
+    <t>296-4940</t>
+  </si>
+  <si>
+    <t>679-5404</t>
+  </si>
+  <si>
+    <t>Connecteur 7 voie</t>
+  </si>
+  <si>
+    <t>Paquet de 10</t>
+  </si>
+  <si>
+    <t>THN 15-1211</t>
+  </si>
+  <si>
+    <t>Traco power 9-18v to 5V 3A</t>
+  </si>
+  <si>
+    <t>438-272</t>
+  </si>
+  <si>
+    <t>Paquet de 20</t>
+  </si>
+  <si>
+    <t>1 en sécu</t>
+  </si>
+  <si>
+    <t>671-4733</t>
+  </si>
+  <si>
+    <t>2N700</t>
+  </si>
+  <si>
+    <t>mosfet N- 200mA</t>
+  </si>
+  <si>
+    <t>sécu</t>
+  </si>
+  <si>
+    <t>PDWorx Paddle shifter</t>
+  </si>
+  <si>
+    <t>palette au volant</t>
   </si>
 </sst>
 </file>
@@ -421,7 +499,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,6 +589,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -518,12 +604,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -549,8 +629,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -651,21 +737,6 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -859,11 +930,80 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -885,10 +1025,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -900,71 +1040,62 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -983,35 +1114,77 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1298,16 +1471,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
     <col min="5" max="5" width="36.5703125" customWidth="1"/>
@@ -1319,253 +1492,255 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="22" t="s">
+      <c r="A1" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="24" t="s">
         <v>9</v>
       </c>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="27" t="s">
+      <c r="A2" s="67" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="29">
+      <c r="F2" s="28">
         <v>1.022</v>
       </c>
-      <c r="G2" s="29">
+      <c r="G2" s="28">
         <f>1.2*F2</f>
         <v>1.2263999999999999</v>
       </c>
-      <c r="H2" s="30">
+      <c r="H2" s="29">
         <v>0.1</v>
       </c>
-      <c r="I2" s="29">
+      <c r="I2" s="28">
         <v>5</v>
       </c>
-      <c r="J2" s="31">
+      <c r="J2" s="30">
         <f>I2*F2*(1-H2)</f>
         <v>4.5990000000000002</v>
       </c>
-      <c r="K2" s="32">
+      <c r="K2" s="31">
         <f>J2*1.2</f>
         <v>5.5187999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="62"/>
-      <c r="B3" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="36" t="s">
+      <c r="A3" s="68"/>
+      <c r="B3" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36">
+      <c r="E3" s="35"/>
+      <c r="F3" s="35">
         <v>20.57</v>
       </c>
-      <c r="G3" s="36">
-        <f t="shared" ref="G3:G24" si="0">1.2*F3</f>
+      <c r="G3" s="35">
+        <f t="shared" ref="G3:G19" si="0">1.2*F3</f>
         <v>24.684000000000001</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="36">
         <v>0.1</v>
       </c>
-      <c r="I3" s="36">
+      <c r="I3" s="35">
         <v>2</v>
       </c>
-      <c r="J3" s="38">
-        <f t="shared" ref="J3:J20" si="1">I3*F3*(1-H3)</f>
+      <c r="J3" s="37">
+        <f t="shared" ref="J3:J19" si="1">I3*F3*(1-H3)</f>
         <v>37.026000000000003</v>
       </c>
-      <c r="K3" s="39">
+      <c r="K3" s="38">
         <f>J3*1.2</f>
         <v>44.431200000000004</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="45">
+      <c r="A4" s="69"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="42">
         <f>SUM(F2:F3)</f>
         <v>21.591999999999999</v>
       </c>
-      <c r="G4" s="45">
+      <c r="G4" s="42">
         <f t="shared" ref="G4:K4" si="2">SUM(G2:G3)</f>
         <v>25.910400000000003</v>
       </c>
-      <c r="H4" s="45">
+      <c r="H4" s="42">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="I4" s="45">
+      <c r="I4" s="42">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="J4" s="45">
+      <c r="J4" s="42">
         <f t="shared" si="2"/>
         <v>41.625</v>
       </c>
-      <c r="K4" s="45">
+      <c r="K4" s="65">
         <f t="shared" si="2"/>
         <v>49.95</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="63" t="s">
-        <v>98</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="11">
+      <c r="A5" s="70" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="28">
         <v>43.46</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="28">
         <f t="shared" si="0"/>
         <v>52.152000000000001</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="29">
         <v>0.05</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="28">
         <v>1</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="30">
         <f t="shared" si="1"/>
         <v>41.286999999999999</v>
       </c>
-      <c r="K5" s="17">
-        <f t="shared" ref="K5:K24" si="3">J5*1.2</f>
+      <c r="K5" s="31">
+        <f t="shared" ref="K5:K19" si="3">J5*1.2</f>
         <v>49.544399999999996</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="63"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54">
+      <c r="A6" s="71"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="65">
         <v>43.46</v>
       </c>
-      <c r="L6" s="55" t="s">
-        <v>96</v>
+      <c r="L6" s="50" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="59"/>
-      <c r="B7" s="46" t="s">
+      <c r="A7" s="72">
+        <v>3</v>
+      </c>
+      <c r="B7" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="57" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7" s="11">
+      <c r="C7" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="14">
         <v>30.97</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="14">
         <f>1.2*F7</f>
         <v>37.163999999999994</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="15">
         <v>0.1</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="14">
         <v>2</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="16">
         <f t="shared" si="1"/>
         <v>55.746000000000002</v>
       </c>
-      <c r="K7" s="17">
+      <c r="K7" s="16">
         <f t="shared" si="3"/>
         <v>66.895200000000003</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="59"/>
-      <c r="B8" s="40" t="s">
+      <c r="A8" s="72"/>
+      <c r="B8" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="48" t="s">
-        <v>75</v>
+      <c r="C8" s="45" t="s">
+        <v>59</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="F8" s="11">
         <v>16</v>
@@ -1590,18 +1765,18 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="59"/>
-      <c r="B9" s="40" t="s">
+      <c r="A9" s="72"/>
+      <c r="B9" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="49" t="s">
-        <v>82</v>
+      <c r="C9" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>66</v>
       </c>
       <c r="F9" s="11">
         <v>16.47</v>
@@ -1626,18 +1801,18 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="59"/>
-      <c r="B10" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="57" t="s">
-        <v>78</v>
+      <c r="A10" s="72"/>
+      <c r="B10" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>62</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="F10" s="14">
         <v>13.59</v>
@@ -1662,25 +1837,25 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="59"/>
-      <c r="B11" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="57" t="s">
-        <v>102</v>
+      <c r="A11" s="72"/>
+      <c r="B11" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>111</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="F11" s="11">
-        <v>0.78900000000000003</v>
+        <v>0.82</v>
       </c>
       <c r="G11" s="11">
         <f t="shared" ref="G11:G14" si="4">1.2*F11</f>
-        <v>0.94679999999999997</v>
+        <v>0.98399999999999987</v>
       </c>
       <c r="H11" s="12">
         <v>0.1</v>
@@ -1690,61 +1865,68 @@
       </c>
       <c r="J11" s="17">
         <f t="shared" ref="J11:J14" si="5">I11*F11*(1-H11)</f>
-        <v>7.1010000000000009</v>
+        <v>7.38</v>
       </c>
       <c r="K11" s="17">
         <f t="shared" ref="K11:K14" si="6">J11*1.2</f>
-        <v>8.5212000000000003</v>
+        <v>8.8559999999999999</v>
       </c>
       <c r="L11" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
-      <c r="B12" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="57" t="s">
-        <v>106</v>
+      <c r="A12" s="72"/>
+      <c r="B12" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>110</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" s="11"/>
+        <v>87</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1.68</v>
+      </c>
       <c r="G12" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.016</v>
       </c>
       <c r="H12" s="12">
         <v>0.1</v>
       </c>
-      <c r="I12" s="11"/>
+      <c r="I12" s="11">
+        <v>5</v>
+      </c>
       <c r="J12" s="17">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7.5600000000000005</v>
       </c>
       <c r="K12" s="17">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>9.072000000000001</v>
+      </c>
+      <c r="L12" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
-      <c r="B13" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>110</v>
+      <c r="A13" s="72"/>
+      <c r="B13" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>89</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="F13" s="11">
         <v>0.27600000000000002</v>
@@ -1768,251 +1950,854 @@
         <v>1.4904000000000002</v>
       </c>
       <c r="L13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="56"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="72"/>
+      <c r="B14" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0.23300000000000001</v>
+      </c>
       <c r="G14" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.27960000000000002</v>
       </c>
       <c r="H14" s="12">
         <v>0.1</v>
       </c>
-      <c r="I14" s="11"/>
+      <c r="I14" s="11">
+        <v>10</v>
+      </c>
       <c r="J14" s="17">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.097</v>
       </c>
       <c r="K14" s="17">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="13"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
+        <v>2.5164</v>
+      </c>
+      <c r="L14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="72"/>
+      <c r="B15" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="11">
+        <v>7.8E-2</v>
+      </c>
       <c r="G15" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.3600000000000003E-2</v>
       </c>
       <c r="H15" s="12">
         <v>0.1</v>
       </c>
-      <c r="I15" s="11"/>
+      <c r="I15" s="11">
+        <v>100</v>
+      </c>
       <c r="J15" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.02</v>
       </c>
       <c r="K15" s="17">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="12">
+        <v>8.4239999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="72"/>
+      <c r="B16" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="57" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" s="35">
+        <v>3.3</v>
+      </c>
+      <c r="G16" s="35">
+        <f t="shared" si="0"/>
+        <v>3.9599999999999995</v>
+      </c>
+      <c r="H16" s="36">
         <v>0.1</v>
       </c>
-      <c r="I16" s="11"/>
-      <c r="J16" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="17">
+      <c r="I16" s="35">
+        <v>1</v>
+      </c>
+      <c r="J16" s="37">
+        <f t="shared" si="1"/>
+        <v>2.9699999999999998</v>
+      </c>
+      <c r="K16" s="37">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="13"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+        <v>3.5639999999999996</v>
+      </c>
+      <c r="L16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="72"/>
+      <c r="B17" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="11">
+        <v>1.022</v>
+      </c>
       <c r="G17" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>1.2*F17</f>
+        <v>1.2263999999999999</v>
       </c>
       <c r="H17" s="12">
         <v>0.1</v>
       </c>
-      <c r="I17" s="11"/>
+      <c r="I17" s="11">
+        <v>5</v>
+      </c>
       <c r="J17" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>I17*F17*(1-H17)</f>
+        <v>4.5990000000000002</v>
       </c>
       <c r="K17" s="17">
+        <f>J17*1.2</f>
+        <v>5.5187999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="72"/>
+      <c r="B18" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" s="14">
+        <v>2.117</v>
+      </c>
+      <c r="G18" s="14">
+        <f t="shared" si="0"/>
+        <v>2.5404</v>
+      </c>
+      <c r="H18" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="I18" s="14">
+        <v>13</v>
+      </c>
+      <c r="J18" s="16">
+        <f t="shared" si="1"/>
+        <v>24.768900000000002</v>
+      </c>
+      <c r="K18" s="16">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="13"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="I18" s="11"/>
-      <c r="J18" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K18" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="13"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+        <v>29.72268</v>
+      </c>
+      <c r="L18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="72"/>
+      <c r="B19" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="11">
+        <v>2.4729999999999999</v>
+      </c>
       <c r="G19" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.9675999999999996</v>
       </c>
       <c r="H19" s="12">
         <v>0.1</v>
       </c>
-      <c r="I19" s="11"/>
+      <c r="I19" s="11">
+        <v>4</v>
+      </c>
       <c r="J19" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.9027999999999992</v>
       </c>
       <c r="K19" s="17">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
+        <v>10.683359999999999</v>
+      </c>
+      <c r="L19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="72"/>
+      <c r="B20" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>114</v>
+      </c>
       <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="F20" s="11">
+        <v>2.6</v>
+      </c>
       <c r="G20" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+        <f t="shared" ref="G20:G37" si="7">1.2*F20</f>
+        <v>3.12</v>
+      </c>
+      <c r="H20" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I20" s="11">
+        <v>3</v>
+      </c>
       <c r="J20" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="J20:J37" si="8">I20*F20*(1-H20)</f>
+        <v>7.0200000000000005</v>
       </c>
       <c r="K20" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="G21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <f t="shared" ref="J21:J24" si="7">I21*F21</f>
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="G22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J22">
+        <f t="shared" ref="K20:K37" si="9">J20*1.2</f>
+        <v>8.4239999999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="72"/>
+      <c r="B21" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" s="11">
+        <v>0.51</v>
+      </c>
+      <c r="G21" s="11">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="G23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J23">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="H21" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I21" s="11">
+        <v>10</v>
+      </c>
+      <c r="J21" s="17">
+        <f t="shared" si="8"/>
+        <v>4.59</v>
+      </c>
+      <c r="K21" s="17">
+        <f t="shared" si="9"/>
+        <v>5.508</v>
+      </c>
+      <c r="L21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="72"/>
+      <c r="B22" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F22" s="11">
+        <v>0.72</v>
+      </c>
+      <c r="G22" s="11">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="G24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J24">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="H22" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I22" s="11">
+        <v>5</v>
+      </c>
+      <c r="J22" s="17">
+        <f t="shared" si="8"/>
+        <v>3.2399999999999998</v>
+      </c>
+      <c r="K22" s="17">
+        <f t="shared" si="9"/>
+        <v>3.8879999999999995</v>
+      </c>
+      <c r="L22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="72"/>
+      <c r="B23" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="11">
+        <v>1.76</v>
+      </c>
+      <c r="G23" s="11">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.1120000000000001</v>
+      </c>
+      <c r="H23" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I23" s="11">
+        <v>5</v>
+      </c>
+      <c r="J23" s="17">
+        <f t="shared" si="8"/>
+        <v>7.9200000000000008</v>
+      </c>
+      <c r="K23" s="17">
+        <f t="shared" si="9"/>
+        <v>9.5040000000000013</v>
+      </c>
+      <c r="L23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="72"/>
+      <c r="B24" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" s="11">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="G24" s="11">
+        <f t="shared" si="7"/>
+        <v>0.2712</v>
+      </c>
+      <c r="H24" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I24" s="11">
+        <v>10</v>
+      </c>
+      <c r="J24" s="17">
+        <f t="shared" si="8"/>
+        <v>2.0340000000000003</v>
+      </c>
+      <c r="K24" s="17">
+        <f t="shared" si="9"/>
+        <v>2.4408000000000003</v>
+      </c>
+      <c r="L24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="72"/>
+      <c r="B25" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" s="11">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="G25" s="11">
+        <f t="shared" si="7"/>
+        <v>0.54239999999999999</v>
+      </c>
+      <c r="H25" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I25" s="11">
+        <v>5</v>
+      </c>
+      <c r="J25" s="17">
+        <f t="shared" si="8"/>
+        <v>2.0340000000000003</v>
+      </c>
+      <c r="K25" s="17">
+        <f t="shared" si="9"/>
+        <v>2.4408000000000003</v>
+      </c>
+      <c r="L25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="72"/>
+      <c r="B26" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" s="11">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="G26" s="11">
+        <f t="shared" si="7"/>
+        <v>0.32280000000000003</v>
+      </c>
+      <c r="H26" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I26" s="11">
+        <v>10</v>
+      </c>
+      <c r="J26" s="17">
+        <f t="shared" si="8"/>
+        <v>2.4210000000000003</v>
+      </c>
+      <c r="K26" s="17">
+        <f t="shared" si="9"/>
+        <v>2.9052000000000002</v>
+      </c>
+      <c r="L26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="72"/>
+      <c r="B27" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F27" s="11">
+        <v>37.340000000000003</v>
+      </c>
+      <c r="G27" s="11">
+        <f t="shared" si="7"/>
+        <v>44.808</v>
+      </c>
+      <c r="H27" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I27" s="11">
+        <v>2</v>
+      </c>
+      <c r="J27" s="17">
+        <f t="shared" si="8"/>
+        <v>67.212000000000003</v>
+      </c>
+      <c r="K27" s="17">
+        <f t="shared" si="9"/>
+        <v>80.654399999999995</v>
+      </c>
+      <c r="L27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="72"/>
+      <c r="B28" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F28" s="11">
+        <v>0.219</v>
+      </c>
+      <c r="G28" s="11">
+        <f t="shared" si="7"/>
+        <v>0.26279999999999998</v>
+      </c>
+      <c r="H28" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I28" s="11">
+        <v>20</v>
+      </c>
+      <c r="J28" s="17">
+        <f t="shared" si="8"/>
+        <v>3.9420000000000002</v>
+      </c>
+      <c r="K28" s="17">
+        <f t="shared" si="9"/>
+        <v>4.7304000000000004</v>
+      </c>
+      <c r="L28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="72"/>
+      <c r="B29" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35">
+        <v>20.57</v>
+      </c>
+      <c r="G29" s="11">
+        <f t="shared" si="7"/>
+        <v>24.684000000000001</v>
+      </c>
+      <c r="H29" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I29" s="11">
+        <v>2</v>
+      </c>
+      <c r="J29" s="17">
+        <f t="shared" si="8"/>
+        <v>37.026000000000003</v>
+      </c>
+      <c r="K29" s="17">
+        <f t="shared" si="9"/>
+        <v>44.431200000000004</v>
+      </c>
+      <c r="L29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="72"/>
+      <c r="B30" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="45"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I30" s="11"/>
+      <c r="J30" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="72"/>
+      <c r="B31" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="45"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I31" s="11"/>
+      <c r="J31" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="72"/>
+      <c r="B32" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="45"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I32" s="11"/>
+      <c r="J32" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="72"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I33" s="11"/>
+      <c r="J33" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="72"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I34" s="11"/>
+      <c r="J34" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="72"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H35" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I35" s="11"/>
+      <c r="J35" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="72"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H36" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I36" s="11"/>
+      <c r="J36" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K36" s="17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="72"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H37" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="I37" s="11"/>
+      <c r="J37" s="17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K37" s="17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="61">
+        <f>SUM(K7:K37)</f>
+        <v>361.41443999999996</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
-          <x14:formula1>
-            <xm:f>Données!$A$1:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B21</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F15CAACE-BD3C-4F3F-8AD7-94DA2B82CEF2}">
           <x14:formula1>
             <xm:f>Données!$A$1:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B6</xm:sqref>
+          <xm:sqref>B2:B6 B17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{21FB2DF8-2938-45F7-9B58-C8E63999EABF}">
           <x14:formula1>
             <xm:f>Données!$A$1:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B7:B20</xm:sqref>
+          <xm:sqref>B7:B16 B18:B37</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2194,22 +2979,22 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2265,14 +3050,14 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>65</v>
+      <c r="A2" s="25" t="s">
+        <v>49</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F2">
         <f>1.2*E2</f>
@@ -2288,37 +3073,37 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="42"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="45">
+      <c r="A3" s="40"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="42">
         <f>SUM(E1:E2)</f>
         <v>0</v>
       </c>
-      <c r="F3" s="45">
+      <c r="F3" s="42">
         <f t="shared" ref="F3:I3" si="0">SUM(F1:F2)</f>
         <v>0</v>
       </c>
-      <c r="G3" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H3" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I3" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J3" s="58">
+      <c r="G3" s="42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H3" s="42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I3" s="42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J3" s="53">
         <v>35.22</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2342,8 +3127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2389,361 +3174,346 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2">
-        <v>54.72</v>
-      </c>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="25"/>
+      <c r="B2" s="54"/>
+      <c r="D2" s="33"/>
       <c r="F2">
-        <f>1.2*E2</f>
-        <v>65.664000000000001</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
+        <f t="shared" ref="F2" si="0">1.2*E2</f>
+        <v>0</v>
       </c>
       <c r="I2">
-        <f>H2*E2</f>
-        <v>54.72</v>
+        <f t="shared" ref="I2" si="1">H2*E2</f>
+        <v>0</v>
       </c>
       <c r="J2">
-        <f>I2*1.2</f>
-        <v>65.664000000000001</v>
+        <f t="shared" ref="J2" si="2">I2*1.2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
+      <c r="A3" s="25"/>
       <c r="F3">
-        <f t="shared" ref="F3:F24" si="0">1.2*E3</f>
+        <f t="shared" ref="F3:F24" si="3">1.2*E3</f>
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I24" si="1">H3*E3</f>
+        <f t="shared" ref="I3:I24" si="4">H3*E3</f>
         <v>0</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J24" si="2">I3*1.2</f>
+        <f t="shared" ref="J3:J24" si="5">I3*1.2</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
+      <c r="A4" s="25"/>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
+      <c r="A5" s="25"/>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
+      <c r="A6" s="25"/>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
+      <c r="A7" s="25"/>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
+      <c r="A8" s="25"/>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
+      <c r="A9" s="25"/>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
+      <c r="A10" s="25"/>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
+      <c r="A11" s="25"/>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26"/>
+      <c r="A12" s="25"/>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
+      <c r="A13" s="25"/>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
+      <c r="A14" s="25"/>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
+      <c r="A15" s="25"/>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
+      <c r="A16" s="25"/>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
+      <c r="A17" s="25"/>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26"/>
+      <c r="A18" s="25"/>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
+      <c r="A19" s="25"/>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="25"/>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2772,6 +3542,123 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8FBB1F-3B5A-4715-9205-E64014F4A9F8}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="39" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="33"/>
+      <c r="E2" s="11">
+        <f>305.3/1.2</f>
+        <v>254.41666666666669</v>
+      </c>
+      <c r="F2" s="11">
+        <f t="shared" ref="F2:F3" si="0">1.2*E2</f>
+        <v>305.3</v>
+      </c>
+      <c r="G2" s="12">
+        <v>0</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1</v>
+      </c>
+      <c r="I2" s="11">
+        <f t="shared" ref="I2:I3" si="1">H2*E2</f>
+        <v>254.41666666666669</v>
+      </c>
+      <c r="J2" s="11">
+        <f t="shared" ref="J2:J3" si="2">I2*1.2</f>
+        <v>305.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="74"/>
+      <c r="E3" s="76" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3">
+        <f>J2</f>
+        <v>305.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3BEDBA88-8B64-47CE-AF14-F0BC3A3BFFD0}">
+          <x14:formula1>
+            <xm:f>Données!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
@@ -2792,11 +3679,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
       <c r="D1" s="10" t="s">
         <v>42</v>
       </c>
@@ -2925,13 +3812,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -2948,13 +3835,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="E7">
         <v>293</v>
@@ -3240,494 +4127,6 @@
             <xm:f>Données!$A$1:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A22</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2975CF6-F759-4AB5-BD70-F4541FA768DC}">
-  <dimension ref="A1:K24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2">
-        <f>1.2*E2</f>
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <f>H2*E2</f>
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <f>I2*1.2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F24" si="0">1.2*E3</f>
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I24" si="1">H3*E3</f>
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J24" si="2">I3*1.2</f>
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
-      <c r="C6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26"/>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26"/>
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4380C4A4-E62E-475A-A73D-70090E7E2E9A}">
-          <x14:formula1>
-            <xm:f>Données!$A$1:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>A21</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5B58D1E6-4568-4AB6-9373-5555FB956C9D}">
-          <x14:formula1>
-            <xm:f>Données!$A$1:$A$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2:A20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3788,11 +4187,11 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="51" t="s">
-        <v>84</v>
+      <c r="B2" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>68</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>17</v>
@@ -4255,34 +4654,34 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="42"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="45">
+      <c r="A5" s="40"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="42">
         <f>SUM(E3:E4)</f>
         <v>0</v>
       </c>
-      <c r="F5" s="45">
+      <c r="F5" s="42">
         <f t="shared" ref="F5:I5" si="3">SUM(F3:F4)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="45">
+      <c r="G5" s="42">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H5" s="45">
+      <c r="H5" s="42">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I5" s="45">
+      <c r="I5" s="42">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J5" s="45" t="s">
-        <v>92</v>
+      <c r="J5" s="42" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -4610,10 +5009,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="52" t="s">
+      <c r="A2" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="49" t="s">
         <v>33</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -4633,8 +5032,8 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
-        <v>66</v>
+      <c r="A3" s="25" t="s">
+        <v>50</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>34</v>
@@ -4656,8 +5055,8 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
-        <v>66</v>
+      <c r="A4" s="25" t="s">
+        <v>50</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>35</v>
@@ -4679,8 +5078,8 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
-        <v>66</v>
+      <c r="A5" s="25" t="s">
+        <v>50</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>37</v>
@@ -4702,8 +5101,8 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
-        <v>66</v>
+      <c r="A6" s="25" t="s">
+        <v>50</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
@@ -4725,7 +5124,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
+      <c r="A7" s="25"/>
       <c r="F7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4740,7 +5139,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
+      <c r="A8" s="25"/>
       <c r="F8">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4755,7 +5154,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
+      <c r="A9" s="25"/>
       <c r="F9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4770,7 +5169,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
+      <c r="A10" s="25"/>
       <c r="F10">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4785,7 +5184,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
+      <c r="A11" s="25"/>
       <c r="F11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4800,7 +5199,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26"/>
+      <c r="A12" s="25"/>
       <c r="F12">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4815,7 +5214,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
+      <c r="A13" s="25"/>
       <c r="F13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4830,7 +5229,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
+      <c r="A14" s="25"/>
       <c r="F14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4845,7 +5244,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
+      <c r="A15" s="25"/>
       <c r="F15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4860,7 +5259,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
+      <c r="A16" s="25"/>
       <c r="F16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4875,7 +5274,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
+      <c r="A17" s="25"/>
       <c r="F17">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4890,7 +5289,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26"/>
+      <c r="A18" s="25"/>
       <c r="F18">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4905,7 +5304,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
+      <c r="A19" s="25"/>
       <c r="F19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4920,7 +5319,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="25"/>
       <c r="F20">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
MEP adaptateur pression d'huile
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Commandes.xlsx
+++ b/EL - Electrical/Autre/Commandes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\EL - Electrical\Autre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9BD2D5-83F1-4DC3-998D-A5C447E9D33A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3E02EA-DCC7-4F1F-B04B-8FD07A86AB45}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS components" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="256">
-  <si>
-    <t>numéro de la commande</t>
-  </si>
   <si>
     <t>Système</t>
   </si>
@@ -854,6 +851,9 @@
   </si>
   <si>
     <t>Diamètre de 24mm</t>
+  </si>
+  <si>
+    <t>Numéro de la commande</t>
   </si>
 </sst>
 </file>
@@ -1875,18 +1875,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1909,6 +1897,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1918,29 +1930,17 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2343,8 +2343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2366,57 +2366,57 @@
   <sheetData>
     <row r="1" spans="1:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="61" t="s">
+      <c r="L1" s="62" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="123" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="62" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="124" t="s">
+      <c r="B2" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="126" t="s">
+      <c r="C2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="F2" s="9">
         <v>1.022</v>
@@ -2441,15 +2441,15 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="124"/>
-      <c r="B3" s="127" t="s">
+      <c r="A3" s="123"/>
+      <c r="B3" s="119" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="14" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>18</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="14">
@@ -2475,12 +2475,12 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="124"/>
-      <c r="B4" s="123"/>
+      <c r="A4" s="123"/>
+      <c r="B4" s="116"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
       <c r="E4" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="21">
         <f t="shared" ref="F4:K4" si="0">SUM(F2:F3)</f>
@@ -2507,24 +2507,24 @@
         <v>49.95</v>
       </c>
       <c r="L4" s="60" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="123" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="117" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="125" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="F5" s="9">
         <v>43.46</v>
@@ -2549,12 +2549,12 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="124"/>
-      <c r="B6" s="123"/>
+      <c r="A6" s="123"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
@@ -2565,24 +2565,24 @@
         <v>43.46</v>
       </c>
       <c r="L6" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="120">
+      <c r="A7" s="124">
         <v>3</v>
       </c>
       <c r="B7" s="98" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="94" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="79" t="s">
         <v>50</v>
-      </c>
-      <c r="E7" s="79" t="s">
-        <v>51</v>
       </c>
       <c r="F7" s="79">
         <v>0.23300000000000001</v>
@@ -2606,22 +2606,22 @@
         <v>2.5164</v>
       </c>
       <c r="L7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="125"/>
+      <c r="B8" s="99" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="34" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="121"/>
-      <c r="B8" s="99" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="34" t="s">
+      <c r="D8" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="E8" s="29" t="s">
         <v>54</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>55</v>
       </c>
       <c r="F8" s="29">
         <v>7.8E-2</v>
@@ -2645,22 +2645,22 @@
         <v>8.4239999999999995</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="121"/>
+      <c r="A9" s="125"/>
       <c r="B9" s="100" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="D9" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="E9" s="33" t="s">
         <v>14</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>15</v>
       </c>
       <c r="F9" s="29">
         <v>1.022</v>
@@ -2685,18 +2685,18 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="121"/>
+      <c r="A10" s="125"/>
       <c r="B10" s="101" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="E10" s="25" t="s">
         <v>57</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>58</v>
       </c>
       <c r="F10" s="25">
         <v>2.117</v>
@@ -2720,22 +2720,22 @@
         <v>29.72268</v>
       </c>
       <c r="L10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="125"/>
+      <c r="B11" s="101" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="28" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="121"/>
-      <c r="B11" s="101" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="28" t="s">
+      <c r="D11" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="E11" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>62</v>
       </c>
       <c r="F11" s="29">
         <v>2.4729999999999999</v>
@@ -2759,19 +2759,19 @@
         <v>10.683359999999999</v>
       </c>
       <c r="L11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="121"/>
+      <c r="A12" s="125"/>
       <c r="B12" s="101" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="D12" s="29" t="s">
         <v>247</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>248</v>
       </c>
       <c r="E12" s="25"/>
       <c r="F12" s="25">
@@ -2797,15 +2797,15 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="121"/>
+      <c r="A13" s="125"/>
       <c r="B13" s="101" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="D13" s="29" t="s">
         <v>249</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>250</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="29">
@@ -2831,15 +2831,15 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="121"/>
+      <c r="A14" s="125"/>
       <c r="B14" s="101" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
+        <v>250</v>
+      </c>
+      <c r="D14" s="29" t="s">
         <v>251</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>252</v>
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="25">
@@ -2853,32 +2853,32 @@
         <v>0.1</v>
       </c>
       <c r="I14" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14" s="27">
         <f t="shared" si="5"/>
-        <v>22.878000000000004</v>
+        <v>11.439000000000002</v>
       </c>
       <c r="K14" s="102">
         <f t="shared" si="6"/>
-        <v>27.453600000000005</v>
+        <v>13.726800000000003</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="121"/>
+      <c r="A15" s="125"/>
       <c r="B15" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="111" t="s">
-        <v>32</v>
+        <v>11</v>
+      </c>
+      <c r="C15" s="107" t="s">
+        <v>31</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="112" t="s">
-        <v>255</v>
-      </c>
-      <c r="F15" s="112">
+        <v>26</v>
+      </c>
+      <c r="E15" s="108" t="s">
+        <v>254</v>
+      </c>
+      <c r="F15" s="108">
         <v>16.47</v>
       </c>
       <c r="G15" s="25">
@@ -2888,28 +2888,28 @@
       <c r="H15" s="36">
         <v>0.1</v>
       </c>
-      <c r="I15" s="112">
-        <v>1</v>
+      <c r="I15" s="108">
+        <v>2</v>
       </c>
       <c r="J15" s="27">
         <f t="shared" ref="J15" si="7">I15*F15*(1-H15)</f>
-        <v>14.822999999999999</v>
+        <v>29.645999999999997</v>
       </c>
       <c r="K15" s="102">
         <f t="shared" ref="K15" si="8">J15*1.2</f>
-        <v>17.787599999999998</v>
+        <v>35.575199999999995</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="121"/>
+      <c r="A16" s="125"/>
       <c r="B16" s="103" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="92" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="84" t="s">
         <v>82</v>
-      </c>
-      <c r="D16" s="84" t="s">
-        <v>83</v>
       </c>
       <c r="E16" s="84"/>
       <c r="F16" s="84">
@@ -2935,18 +2935,18 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="121"/>
+      <c r="A17" s="125"/>
       <c r="B17" s="93" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="94" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="E17" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="F17" s="9">
         <v>13.59</v>
@@ -2971,18 +2971,18 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="121"/>
+      <c r="A18" s="125"/>
       <c r="B18" s="95" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="E18" s="29" t="s">
         <v>38</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>39</v>
       </c>
       <c r="F18" s="29">
         <v>0.82</v>
@@ -3006,22 +3006,22 @@
         <v>8.8559999999999999</v>
       </c>
       <c r="L18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="125"/>
+      <c r="B19" s="95" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="28" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="121"/>
-      <c r="B19" s="95" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="28" t="s">
+      <c r="D19" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="E19" s="29" t="s">
         <v>42</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>43</v>
       </c>
       <c r="F19" s="29">
         <v>1.68</v>
@@ -3045,22 +3045,22 @@
         <v>9.072000000000001</v>
       </c>
       <c r="L19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="125"/>
+      <c r="B20" s="95" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="34" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="121"/>
-      <c r="B20" s="95" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="34" t="s">
+      <c r="D20" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="E20" s="29" t="s">
         <v>46</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>47</v>
       </c>
       <c r="F20" s="29">
         <v>0.27600000000000002</v>
@@ -3084,19 +3084,19 @@
         <v>1.4904000000000002</v>
       </c>
       <c r="L20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="121"/>
+      <c r="A21" s="125"/>
       <c r="B21" s="96" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="29" t="s">
         <v>64</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>65</v>
       </c>
       <c r="E21" s="29"/>
       <c r="F21" s="29">
@@ -3122,18 +3122,18 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="121"/>
+      <c r="A22" s="125"/>
       <c r="B22" s="96" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F22" s="29">
         <v>0.72</v>
@@ -3157,22 +3157,22 @@
         <v>3.8879999999999995</v>
       </c>
       <c r="L22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="121"/>
+      <c r="A23" s="125"/>
       <c r="B23" s="96" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F23" s="29">
         <v>0.45200000000000001</v>
@@ -3196,22 +3196,22 @@
         <v>4.8816000000000006</v>
       </c>
       <c r="L23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="121"/>
+      <c r="A24" s="125"/>
       <c r="B24" s="96" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="E24" s="29" t="s">
         <v>74</v>
-      </c>
-      <c r="E24" s="29" t="s">
-        <v>75</v>
       </c>
       <c r="F24" s="29">
         <v>37.340000000000003</v>
@@ -3235,22 +3235,22 @@
         <v>80.654399999999995</v>
       </c>
       <c r="L24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="125"/>
+      <c r="B25" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="28" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="121"/>
-      <c r="B25" s="96" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="28" t="s">
+      <c r="D25" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="E25" s="29" t="s">
         <v>78</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>79</v>
       </c>
       <c r="F25" s="29">
         <v>0.219</v>
@@ -3274,19 +3274,19 @@
         <v>4.7304000000000004</v>
       </c>
       <c r="L25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="121"/>
+      <c r="A26" s="125"/>
       <c r="B26" s="97" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="92" t="s">
+      <c r="D26" s="84" t="s">
         <v>17</v>
-      </c>
-      <c r="D26" s="84" t="s">
-        <v>18</v>
       </c>
       <c r="E26" s="84"/>
       <c r="F26" s="84">
@@ -3311,19 +3311,19 @@
         <v>44.431200000000004</v>
       </c>
       <c r="L26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="121"/>
+      <c r="A27" s="125"/>
       <c r="B27" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="78" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="78" t="s">
+      <c r="D27" s="79" t="s">
         <v>85</v>
-      </c>
-      <c r="D27" s="79" t="s">
-        <v>86</v>
       </c>
       <c r="E27" s="79"/>
       <c r="F27" s="79">
@@ -3349,15 +3349,15 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="121"/>
+      <c r="A28" s="125"/>
       <c r="B28" s="80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C28" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="29" t="s">
         <v>87</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>88</v>
       </c>
       <c r="E28" s="29"/>
       <c r="F28" s="29">
@@ -3382,19 +3382,19 @@
         <v>2.7864</v>
       </c>
       <c r="L28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="125"/>
+      <c r="B29" s="80" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="28" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="121"/>
-      <c r="B29" s="80" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="28" t="s">
+      <c r="D29" s="29" t="s">
         <v>90</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>91</v>
       </c>
       <c r="E29" s="29"/>
       <c r="F29" s="29">
@@ -3419,22 +3419,22 @@
         <v>2.9268000000000001</v>
       </c>
       <c r="L29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="121"/>
+      <c r="A30" s="125"/>
       <c r="B30" s="80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C30" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="D30" s="29" t="s">
-        <v>93</v>
-      </c>
       <c r="E30" s="29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F30" s="29">
         <v>1.1100000000000001</v>
@@ -3459,15 +3459,15 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="121"/>
+      <c r="A31" s="125"/>
       <c r="B31" s="80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C31" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="37" t="s">
         <v>94</v>
-      </c>
-      <c r="D31" s="37" t="s">
-        <v>95</v>
       </c>
       <c r="E31" s="29"/>
       <c r="F31" s="29">
@@ -3493,15 +3493,15 @@
       </c>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="121"/>
+      <c r="A32" s="125"/>
       <c r="B32" s="80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C32" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="29" t="s">
         <v>96</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>97</v>
       </c>
       <c r="E32" s="29"/>
       <c r="F32" s="29">
@@ -3526,19 +3526,19 @@
         <v>9.072000000000001</v>
       </c>
       <c r="L32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="125"/>
+      <c r="B33" s="80" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="32" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="121"/>
-      <c r="B33" s="80" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="32" t="s">
+      <c r="D33" s="33" t="s">
         <v>99</v>
-      </c>
-      <c r="D33" s="33" t="s">
-        <v>100</v>
       </c>
       <c r="E33" s="29"/>
       <c r="F33" s="29">
@@ -3563,19 +3563,19 @@
         <v>5.7239999999999993</v>
       </c>
       <c r="L33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="125"/>
+      <c r="B34" s="80" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="28" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="121"/>
-      <c r="B34" s="80" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" s="28" t="s">
+      <c r="D34" s="29" t="s">
         <v>102</v>
-      </c>
-      <c r="D34" s="29" t="s">
-        <v>103</v>
       </c>
       <c r="E34" s="29"/>
       <c r="F34" s="29">
@@ -3600,22 +3600,22 @@
         <v>6.4259999999999993</v>
       </c>
       <c r="L34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="121"/>
+      <c r="A35" s="125"/>
       <c r="B35" s="80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C35" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="D35" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="D35" s="29" t="s">
-        <v>223</v>
-      </c>
       <c r="E35" s="29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F35" s="29">
         <v>0.254</v>
@@ -3639,22 +3639,22 @@
         <v>2.7431999999999999</v>
       </c>
       <c r="L35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="121"/>
+      <c r="A36" s="125"/>
       <c r="B36" s="80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C36" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="E36" s="29" t="s">
         <v>229</v>
-      </c>
-      <c r="D36" s="29" t="s">
-        <v>223</v>
-      </c>
-      <c r="E36" s="29" t="s">
-        <v>230</v>
       </c>
       <c r="F36" s="29">
         <v>0.85799999999999998</v>
@@ -3679,15 +3679,15 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="121"/>
+      <c r="A37" s="125"/>
       <c r="B37" s="80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C37" s="76" t="s">
+        <v>230</v>
+      </c>
+      <c r="D37" s="29" t="s">
         <v>231</v>
-      </c>
-      <c r="D37" s="29" t="s">
-        <v>232</v>
       </c>
       <c r="E37" s="29"/>
       <c r="F37" s="29">
@@ -3712,19 +3712,19 @@
         <v>1.296</v>
       </c>
       <c r="L37" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="125"/>
+      <c r="B38" s="80" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="76" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="121"/>
-      <c r="B38" s="80" t="s">
-        <v>84</v>
-      </c>
-      <c r="C38" s="76" t="s">
+      <c r="D38" s="29" t="s">
         <v>234</v>
-      </c>
-      <c r="D38" s="29" t="s">
-        <v>235</v>
       </c>
       <c r="E38" s="29"/>
       <c r="F38" s="29">
@@ -3749,19 +3749,19 @@
         <v>1.458</v>
       </c>
       <c r="L38" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="121"/>
+      <c r="A39" s="125"/>
       <c r="B39" s="80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C39" s="76" t="s">
+        <v>235</v>
+      </c>
+      <c r="D39" s="29" t="s">
         <v>236</v>
-      </c>
-      <c r="D39" s="29" t="s">
-        <v>237</v>
       </c>
       <c r="E39" s="29"/>
       <c r="F39" s="29">
@@ -3786,19 +3786,19 @@
         <v>1.458</v>
       </c>
       <c r="L39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="121"/>
+      <c r="A40" s="125"/>
       <c r="B40" s="80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C40" s="76" t="s">
+        <v>237</v>
+      </c>
+      <c r="D40" s="29" t="s">
         <v>238</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>239</v>
       </c>
       <c r="E40" s="29"/>
       <c r="F40" s="29">
@@ -3823,19 +3823,19 @@
         <v>1.8900000000000001</v>
       </c>
       <c r="L40" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="121"/>
+      <c r="A41" s="125"/>
       <c r="B41" s="80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C41" s="76" t="s">
+        <v>239</v>
+      </c>
+      <c r="D41" s="29" t="s">
         <v>240</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>241</v>
       </c>
       <c r="E41" s="29"/>
       <c r="F41" s="29">
@@ -3860,19 +3860,19 @@
         <v>1.9979999999999998</v>
       </c>
       <c r="L41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="121"/>
+      <c r="A42" s="125"/>
       <c r="B42" s="80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C42" s="76" t="s">
+        <v>241</v>
+      </c>
+      <c r="D42" s="29" t="s">
         <v>242</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>243</v>
       </c>
       <c r="E42" s="29"/>
       <c r="F42" s="29">
@@ -3897,19 +3897,19 @@
         <v>8.5860000000000003</v>
       </c>
       <c r="L42" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="121"/>
+      <c r="A43" s="125"/>
       <c r="B43" s="82" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C43" s="83" t="s">
+        <v>243</v>
+      </c>
+      <c r="D43" s="84" t="s">
         <v>244</v>
-      </c>
-      <c r="D43" s="84" t="s">
-        <v>245</v>
       </c>
       <c r="E43" s="84"/>
       <c r="F43" s="84">
@@ -3934,22 +3934,22 @@
         <v>6.9660000000000002</v>
       </c>
       <c r="L43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="121"/>
-      <c r="B44" s="115" t="s">
-        <v>198</v>
-      </c>
-      <c r="C44" s="113" t="s">
+      <c r="A44" s="125"/>
+      <c r="B44" s="111" t="s">
+        <v>197</v>
+      </c>
+      <c r="C44" s="109" t="s">
+        <v>252</v>
+      </c>
+      <c r="D44" s="110" t="s">
         <v>253</v>
       </c>
-      <c r="D44" s="114" t="s">
-        <v>254</v>
-      </c>
-      <c r="E44" s="114"/>
-      <c r="F44" s="114">
+      <c r="E44" s="110"/>
+      <c r="F44" s="110">
         <v>16.28</v>
       </c>
       <c r="G44" s="14">
@@ -3959,7 +3959,7 @@
       <c r="H44" s="15">
         <v>0.1</v>
       </c>
-      <c r="I44" s="114">
+      <c r="I44" s="110">
         <v>1</v>
       </c>
       <c r="J44" s="16">
@@ -3972,15 +3972,15 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="121"/>
-      <c r="B45" s="116" t="s">
-        <v>198</v>
+      <c r="A45" s="125"/>
+      <c r="B45" s="112" t="s">
+        <v>197</v>
       </c>
       <c r="C45" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="D45" s="29" t="s">
         <v>215</v>
-      </c>
-      <c r="D45" s="29" t="s">
-        <v>216</v>
       </c>
       <c r="E45" s="29"/>
       <c r="F45" s="29">
@@ -4005,22 +4005,22 @@
         <v>2.4408000000000003</v>
       </c>
       <c r="L45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="121"/>
+      <c r="A46" s="125"/>
       <c r="B46" s="88" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F46" s="29">
         <v>0.105</v>
@@ -4045,18 +4045,18 @@
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="121"/>
+      <c r="A47" s="125"/>
       <c r="B47" s="88" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F47" s="29">
         <v>0.51</v>
@@ -4081,18 +4081,18 @@
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="121"/>
+      <c r="A48" s="125"/>
       <c r="B48" s="88" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F48" s="29">
         <v>2.54</v>
@@ -4116,22 +4116,22 @@
         <v>2.7431999999999999</v>
       </c>
       <c r="L48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="121"/>
+      <c r="A49" s="125"/>
       <c r="B49" s="91" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C49" s="92" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D49" s="84" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E49" s="84" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F49" s="84">
         <v>1.76</v>
@@ -4156,18 +4156,18 @@
       </c>
     </row>
     <row r="50" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="121"/>
+      <c r="A50" s="125"/>
       <c r="B50" s="104" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="C50" s="94" t="s">
+      <c r="D50" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="E50" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="F50" s="9">
         <v>30.97</v>
@@ -4192,18 +4192,18 @@
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="121"/>
+      <c r="A51" s="125"/>
       <c r="B51" s="105" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C51" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D51" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D51" s="29" t="s">
+      <c r="E51" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="E51" s="29" t="s">
-        <v>31</v>
       </c>
       <c r="F51" s="29">
         <v>16</v>
@@ -4228,18 +4228,18 @@
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="121"/>
+      <c r="A52" s="125"/>
       <c r="B52" s="105" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C52" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D52" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E52" s="106" t="s">
         <v>32</v>
-      </c>
-      <c r="D52" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="E52" s="110" t="s">
-        <v>33</v>
       </c>
       <c r="F52" s="29">
         <v>16.47</v>
@@ -4264,15 +4264,15 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="121"/>
+      <c r="A53" s="125"/>
       <c r="B53" s="105" t="s">
-        <v>25</v>
-      </c>
-      <c r="C53" s="128" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" s="120" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53" s="33" t="s">
         <v>104</v>
-      </c>
-      <c r="D53" s="33" t="s">
-        <v>105</v>
       </c>
       <c r="E53" s="29"/>
       <c r="F53" s="38">
@@ -4298,15 +4298,15 @@
       </c>
     </row>
     <row r="54" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="121"/>
+      <c r="A54" s="125"/>
       <c r="B54" s="105" t="s">
-        <v>25</v>
-      </c>
-      <c r="C54" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" s="121" t="s">
+        <v>105</v>
+      </c>
+      <c r="D54" s="33" t="s">
         <v>106</v>
-      </c>
-      <c r="D54" s="33" t="s">
-        <v>107</v>
       </c>
       <c r="E54" s="29"/>
       <c r="F54" s="38">
@@ -4331,19 +4331,19 @@
         <v>2.052</v>
       </c>
       <c r="L54" s="39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="125"/>
+      <c r="B55" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="121" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="121"/>
-      <c r="B55" s="105" t="s">
-        <v>25</v>
-      </c>
-      <c r="C55" s="129" t="s">
+      <c r="D55" s="33" t="s">
         <v>109</v>
-      </c>
-      <c r="D55" s="33" t="s">
-        <v>110</v>
       </c>
       <c r="E55" s="29"/>
       <c r="F55" s="38">
@@ -4368,19 +4368,19 @@
         <v>3.8879999999999995</v>
       </c>
       <c r="L55" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="121"/>
+      <c r="A56" s="125"/>
       <c r="B56" s="105" t="s">
-        <v>25</v>
-      </c>
-      <c r="C56" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56" s="121" t="s">
+        <v>110</v>
+      </c>
+      <c r="D56" s="33" t="s">
         <v>111</v>
-      </c>
-      <c r="D56" s="33" t="s">
-        <v>112</v>
       </c>
       <c r="E56" s="29"/>
       <c r="F56" s="38">
@@ -4405,19 +4405,19 @@
         <v>5.13</v>
       </c>
       <c r="L56" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="121"/>
+      <c r="A57" s="125"/>
       <c r="B57" s="105" t="s">
-        <v>25</v>
-      </c>
-      <c r="C57" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="121" t="s">
+        <v>112</v>
+      </c>
+      <c r="D57" s="33" t="s">
         <v>113</v>
-      </c>
-      <c r="D57" s="33" t="s">
-        <v>114</v>
       </c>
       <c r="E57" s="29"/>
       <c r="F57" s="38">
@@ -4443,15 +4443,15 @@
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="121"/>
+      <c r="A58" s="125"/>
       <c r="B58" s="105" t="s">
-        <v>25</v>
-      </c>
-      <c r="C58" s="129" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="121" t="s">
+        <v>114</v>
+      </c>
+      <c r="D58" s="33" t="s">
         <v>115</v>
-      </c>
-      <c r="D58" s="33" t="s">
-        <v>116</v>
       </c>
       <c r="E58" s="29"/>
       <c r="F58" s="38">
@@ -4477,15 +4477,15 @@
       </c>
     </row>
     <row r="59" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="122"/>
+      <c r="A59" s="126"/>
       <c r="B59" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="130" t="s">
-        <v>117</v>
+        <v>24</v>
+      </c>
+      <c r="C59" s="122" t="s">
+        <v>116</v>
       </c>
       <c r="D59" s="90" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E59" s="84"/>
       <c r="F59" s="84">
@@ -4510,21 +4510,21 @@
         <v>8.4239999999999995</v>
       </c>
       <c r="L59" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E60" s="117" t="s">
-        <v>19</v>
-      </c>
-      <c r="F60" s="118"/>
-      <c r="G60" s="118"/>
-      <c r="H60" s="118"/>
-      <c r="I60" s="118"/>
-      <c r="J60" s="118"/>
-      <c r="K60" s="119">
+      <c r="E60" s="113" t="s">
+        <v>18</v>
+      </c>
+      <c r="F60" s="114"/>
+      <c r="G60" s="114"/>
+      <c r="H60" s="114"/>
+      <c r="I60" s="114"/>
+      <c r="J60" s="114"/>
+      <c r="K60" s="115">
         <f>SUM(K7:K59)</f>
-        <v>643.81284000000005</v>
+        <v>647.87364000000002</v>
       </c>
     </row>
   </sheetData>
@@ -4592,45 +4592,45 @@
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="E1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="H1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="I1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="J1" s="44" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="44" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" s="50" t="s">
         <v>198</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="D2" s="39" t="s">
         <v>199</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>200</v>
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F24" si="0">1.2*E2</f>
@@ -4647,13 +4647,13 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3" s="39" t="s">
         <v>201</v>
-      </c>
-      <c r="D3" s="39" t="s">
-        <v>202</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
@@ -4670,13 +4670,13 @@
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C4" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" s="39" t="s">
         <v>203</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>204</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
@@ -4693,13 +4693,13 @@
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C5" s="50" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5" s="39" t="s">
         <v>205</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>206</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -4716,13 +4716,13 @@
     </row>
     <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D6" s="39" t="s">
         <v>207</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>208</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -5054,39 +5054,39 @@
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="E1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="H1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="I1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="J1" s="44" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="44" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F24" si="0">1.2*E2</f>
@@ -5103,7 +5103,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
@@ -5120,7 +5120,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
@@ -5137,7 +5137,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -5154,7 +5154,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -5171,7 +5171,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
@@ -5188,7 +5188,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
@@ -5205,7 +5205,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
@@ -5222,7 +5222,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
@@ -5239,7 +5239,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
@@ -5489,45 +5489,45 @@
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="E1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="H1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="I1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="J1" s="44" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="44" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" s="39" t="s">
         <v>209</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="D2" t="s">
         <v>210</v>
-      </c>
-      <c r="D2" t="s">
-        <v>211</v>
       </c>
       <c r="F2">
         <f>1.2*E2</f>
@@ -5642,32 +5642,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="63" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="66" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="68" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -5701,34 +5701,34 @@
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="E1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="H1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="I1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="J1" s="44" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="44" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -5737,10 +5737,10 @@
         <v>2313118</v>
       </c>
       <c r="C2" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="39" t="s">
         <v>119</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>120</v>
       </c>
       <c r="E2" s="46">
         <v>3.17</v>
@@ -5769,7 +5769,7 @@
         <v>488203</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3" s="47"/>
       <c r="E3" s="46">
@@ -6004,45 +6004,45 @@
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="E1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="H1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="I1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="J1" s="44" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="44" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" t="s">
         <v>122</v>
-      </c>
-      <c r="D2" t="s">
-        <v>123</v>
       </c>
       <c r="F2">
         <f>1.2*E2</f>
@@ -6062,7 +6062,7 @@
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="21">
         <f>SUM(E1:E2)</f>
@@ -6088,7 +6088,7 @@
         <v>35.22</v>
       </c>
       <c r="K3" s="39" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -6137,48 +6137,48 @@
   <sheetData>
     <row r="1" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="C1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="E1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="H1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="I1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="J1" s="44" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="44" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="D2" s="24" t="s">
         <v>126</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>127</v>
       </c>
       <c r="E2" s="74">
         <v>0.25</v>
@@ -6197,19 +6197,19 @@
         <v>0</v>
       </c>
       <c r="K2" s="39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E3" s="38">
         <v>21.23</v>
@@ -6231,14 +6231,14 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E4" s="38">
         <v>0.19</v>
@@ -6260,14 +6260,14 @@
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E5" s="38">
         <v>0.22</v>
@@ -6286,19 +6286,19 @@
         <v>6.54</v>
       </c>
       <c r="K5" s="39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E6" s="38">
         <v>0.39</v>
@@ -6317,19 +6317,19 @@
         <v>11.67</v>
       </c>
       <c r="K6" s="39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E7" s="38">
         <v>0.22</v>
@@ -6348,19 +6348,19 @@
         <v>6.57</v>
       </c>
       <c r="K7" s="39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E8" s="38">
         <v>0.24</v>
@@ -6379,19 +6379,19 @@
         <v>7.23</v>
       </c>
       <c r="K8" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E9" s="38">
         <v>0.23</v>
@@ -6410,18 +6410,18 @@
         <v>6.87</v>
       </c>
       <c r="K9" s="39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="33" t="s">
         <v>148</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>149</v>
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="38">
@@ -6444,13 +6444,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="33" t="s">
         <v>150</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>151</v>
       </c>
       <c r="D11" s="29"/>
       <c r="E11" s="38">
@@ -6473,13 +6473,13 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="33" t="s">
         <v>152</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>153</v>
       </c>
       <c r="D12" s="29"/>
       <c r="E12" s="38">
@@ -6502,13 +6502,13 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" s="33" t="s">
         <v>154</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>155</v>
       </c>
       <c r="D13" s="29"/>
       <c r="E13" s="38">
@@ -6531,13 +6531,13 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" s="33" t="s">
         <v>156</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>157</v>
       </c>
       <c r="D14" s="29"/>
       <c r="E14" s="38">
@@ -6560,14 +6560,14 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C15" s="29"/>
       <c r="D15" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E15" s="38">
         <v>3.19</v>
@@ -6596,14 +6596,14 @@
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="45"/>
-      <c r="E17" s="106" t="s">
-        <v>221</v>
-      </c>
-      <c r="F17" s="106"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="107">
+      <c r="E17" s="127" t="s">
+        <v>220</v>
+      </c>
+      <c r="F17" s="127"/>
+      <c r="G17" s="127"/>
+      <c r="H17" s="127"/>
+      <c r="I17" s="127"/>
+      <c r="J17" s="128">
         <f>SUM(J2:J15)</f>
         <v>101.52000000000001</v>
       </c>
@@ -6611,12 +6611,12 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="45"/>
-      <c r="E18" s="106"/>
-      <c r="F18" s="106"/>
-      <c r="G18" s="106"/>
-      <c r="H18" s="106"/>
-      <c r="I18" s="106"/>
-      <c r="J18" s="107"/>
+      <c r="E18" s="127"/>
+      <c r="F18" s="127"/>
+      <c r="G18" s="127"/>
+      <c r="H18" s="127"/>
+      <c r="I18" s="127"/>
+      <c r="J18" s="128"/>
       <c r="K18" s="47"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -6654,8 +6654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6669,45 +6669,45 @@
   <sheetData>
     <row r="1" spans="1:10" ht="39" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="53" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>160</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>161</v>
       </c>
       <c r="D2" s="33"/>
       <c r="E2" s="29">
@@ -6735,13 +6735,13 @@
     </row>
     <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="54"/>
-      <c r="E3" s="108" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
+      <c r="E3" s="129" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
       <c r="J3">
         <f>J2</f>
         <v>305.3</v>
@@ -6794,59 +6794,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="130" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="55" t="s">
         <v>162</v>
-      </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="55" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="C2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="D2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="E2" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="F2" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="G2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="H2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="I2" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="J2" s="44" t="s">
         <v>9</v>
-      </c>
-      <c r="J2" s="44" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" t="s">
         <v>164</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>165</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>166</v>
-      </c>
-      <c r="D3" t="s">
-        <v>167</v>
       </c>
       <c r="E3">
         <v>81</v>
@@ -6870,13 +6870,13 @@
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="47"/>
       <c r="B4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" t="s">
         <v>168</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="39" t="s">
         <v>169</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>170</v>
       </c>
       <c r="E4">
         <v>110</v>
@@ -6900,13 +6900,13 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
       <c r="B5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" t="s">
         <v>171</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>172</v>
-      </c>
-      <c r="D5" t="s">
-        <v>173</v>
       </c>
       <c r="E5">
         <v>110</v>
@@ -6930,13 +6930,13 @@
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
       <c r="B6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" t="s">
         <v>174</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>175</v>
-      </c>
-      <c r="D6" t="s">
-        <v>176</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -6954,13 +6954,13 @@
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" t="s">
         <v>177</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>178</v>
-      </c>
-      <c r="D7" t="s">
-        <v>179</v>
       </c>
       <c r="E7">
         <v>293</v>
@@ -7293,48 +7293,48 @@
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="E1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="H1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="I1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="J1" s="44" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="44" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" s="56" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="D2" s="39" t="s">
         <v>181</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>182</v>
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F24" si="0">1.2*E2</f>
@@ -7719,48 +7719,48 @@
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="E1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="H1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="I1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="J1" s="44" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="44" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="F2" s="58" t="s">
         <v>184</v>
-      </c>
-      <c r="F2" s="58" t="s">
-        <v>185</v>
       </c>
       <c r="G2" s="39"/>
       <c r="H2">
@@ -7773,16 +7773,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="39">
         <v>6329</v>
       </c>
       <c r="C3" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3" s="58" t="s">
         <v>186</v>
-      </c>
-      <c r="F3" s="58" t="s">
-        <v>187</v>
       </c>
       <c r="G3" s="39"/>
       <c r="H3">
@@ -7795,16 +7795,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="39" t="s">
         <v>188</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="F4" s="58" t="s">
         <v>189</v>
-      </c>
-      <c r="F4" s="58" t="s">
-        <v>190</v>
       </c>
       <c r="G4" s="39"/>
       <c r="H4">
@@ -7857,45 +7857,45 @@
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="E1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="H1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="I1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="J1" s="44" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="44" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" t="s">
         <v>191</v>
-      </c>
-      <c r="D2" t="s">
-        <v>192</v>
       </c>
       <c r="F2">
         <f>1.2*E2</f>
@@ -7912,13 +7912,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="59" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" t="s">
         <v>193</v>
-      </c>
-      <c r="D3" t="s">
-        <v>194</v>
       </c>
       <c r="F3">
         <f>1.2*E3</f>
@@ -7935,13 +7935,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" t="s">
         <v>195</v>
-      </c>
-      <c r="D4" t="s">
-        <v>196</v>
       </c>
       <c r="F4">
         <f>1.2*E4</f>
@@ -7961,7 +7961,7 @@
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="21">
         <f>SUM(E3:E4)</f>
@@ -7984,7 +7984,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Boite BSPD et gabarits
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Commandes.xlsx
+++ b/EL - Electrical/Autre/Commandes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\EL - Electrical\Autre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3E02EA-DCC7-4F1F-B04B-8FD07A86AB45}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EB40B9-32DB-4358-896E-2845D96D3CA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS components" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="257">
   <si>
     <t>Système</t>
   </si>
@@ -854,6 +854,9 @@
   </si>
   <si>
     <t>Numéro de la commande</t>
+  </si>
+  <si>
+    <t>772-1111</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1054,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1628,11 +1631,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1813,9 +1836,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1941,6 +1961,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2341,10 +2379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2403,10 +2441,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="117" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -2441,8 +2479,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="123"/>
-      <c r="B3" s="119" t="s">
+      <c r="A3" s="122"/>
+      <c r="B3" s="118" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="14" t="s">
@@ -2475,8 +2513,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="123"/>
-      <c r="B4" s="116"/>
+      <c r="A4" s="122"/>
+      <c r="B4" s="115"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
       <c r="E4" s="20" t="s">
@@ -2511,10 +2549,10 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="123" t="s">
+      <c r="A5" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="116" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -2549,8 +2587,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="123"/>
-      <c r="B6" s="116"/>
+      <c r="A6" s="122"/>
+      <c r="B6" s="115"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="20" t="s">
@@ -2569,13 +2607,13 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="124">
+      <c r="A7" s="123">
         <v>3</v>
       </c>
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="94" t="s">
+      <c r="C7" s="93" t="s">
         <v>48</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -2588,7 +2626,7 @@
         <v>0.23300000000000001</v>
       </c>
       <c r="G7" s="79">
-        <f t="shared" ref="G7:G59" si="1">1.2*F7</f>
+        <f t="shared" ref="G7:G61" si="1">1.2*F7</f>
         <v>0.27960000000000002</v>
       </c>
       <c r="H7" s="10">
@@ -2598,11 +2636,11 @@
         <v>10</v>
       </c>
       <c r="J7" s="11">
-        <f t="shared" ref="J7:J59" si="2">I7*F7*(1-H7)</f>
+        <f t="shared" ref="J7:J61" si="2">I7*F7*(1-H7)</f>
         <v>2.097</v>
       </c>
       <c r="K7" s="12">
-        <f t="shared" ref="K7:K59" si="3">J7*1.2</f>
+        <f t="shared" ref="K7:K61" si="3">J7*1.2</f>
         <v>2.5164</v>
       </c>
       <c r="L7" t="s">
@@ -2610,8 +2648,8 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="125"/>
-      <c r="B8" s="99" t="s">
+      <c r="A8" s="124"/>
+      <c r="B8" s="98" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="34" t="s">
@@ -2649,8 +2687,8 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="125"/>
-      <c r="B9" s="100" t="s">
+      <c r="A9" s="124"/>
+      <c r="B9" s="99" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="34" t="s">
@@ -2685,8 +2723,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="125"/>
-      <c r="B10" s="101" t="s">
+      <c r="A10" s="124"/>
+      <c r="B10" s="100" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="35" t="s">
@@ -2715,7 +2753,7 @@
         <f t="shared" si="2"/>
         <v>24.768900000000002</v>
       </c>
-      <c r="K10" s="102">
+      <c r="K10" s="101">
         <f t="shared" si="3"/>
         <v>29.72268</v>
       </c>
@@ -2724,8 +2762,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="125"/>
-      <c r="B11" s="101" t="s">
+      <c r="A11" s="124"/>
+      <c r="B11" s="100" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="28" t="s">
@@ -2763,8 +2801,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="125"/>
-      <c r="B12" s="101" t="s">
+      <c r="A12" s="124"/>
+      <c r="B12" s="100" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="28" t="s">
@@ -2791,14 +2829,14 @@
         <f t="shared" ref="J12:J16" si="5">I12*F12*(1-H12)</f>
         <v>21.905999999999999</v>
       </c>
-      <c r="K12" s="102">
+      <c r="K12" s="101">
         <f t="shared" ref="K12:K16" si="6">J12*1.2</f>
         <v>26.287199999999999</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="125"/>
-      <c r="B13" s="101" t="s">
+      <c r="A13" s="124"/>
+      <c r="B13" s="100" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="28" t="s">
@@ -2831,8 +2869,8 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="125"/>
-      <c r="B14" s="101" t="s">
+      <c r="A14" s="124"/>
+      <c r="B14" s="100" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
@@ -2859,26 +2897,26 @@
         <f t="shared" si="5"/>
         <v>11.439000000000002</v>
       </c>
-      <c r="K14" s="102">
+      <c r="K14" s="101">
         <f t="shared" si="6"/>
         <v>13.726800000000003</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="125"/>
-      <c r="B15" s="100" t="s">
+      <c r="A15" s="124"/>
+      <c r="B15" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="107" t="s">
+      <c r="C15" s="106" t="s">
         <v>31</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="108" t="s">
+      <c r="E15" s="107" t="s">
         <v>254</v>
       </c>
-      <c r="F15" s="108">
+      <c r="F15" s="107">
         <v>16.47</v>
       </c>
       <c r="G15" s="25">
@@ -2888,58 +2926,58 @@
       <c r="H15" s="36">
         <v>0.1</v>
       </c>
-      <c r="I15" s="108">
+      <c r="I15" s="107">
         <v>2</v>
       </c>
       <c r="J15" s="27">
         <f t="shared" ref="J15" si="7">I15*F15*(1-H15)</f>
         <v>29.645999999999997</v>
       </c>
-      <c r="K15" s="102">
+      <c r="K15" s="101">
         <f t="shared" ref="K15" si="8">J15*1.2</f>
         <v>35.575199999999995</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="125"/>
-      <c r="B16" s="103" t="s">
+      <c r="A16" s="124"/>
+      <c r="B16" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="92" t="s">
+      <c r="C16" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="84" t="s">
+      <c r="D16" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="84"/>
-      <c r="F16" s="84">
+      <c r="E16" s="83"/>
+      <c r="F16" s="83">
         <v>11.11</v>
       </c>
-      <c r="G16" s="84">
+      <c r="G16" s="83">
         <f t="shared" si="4"/>
         <v>13.331999999999999</v>
       </c>
-      <c r="H16" s="85">
+      <c r="H16" s="84">
         <v>0.1</v>
       </c>
-      <c r="I16" s="84">
+      <c r="I16" s="83">
         <v>1</v>
       </c>
-      <c r="J16" s="86">
+      <c r="J16" s="85">
         <f t="shared" si="5"/>
         <v>9.9990000000000006</v>
       </c>
-      <c r="K16" s="87">
+      <c r="K16" s="86">
         <f t="shared" si="6"/>
         <v>11.998800000000001</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="125"/>
-      <c r="B17" s="93" t="s">
+      <c r="A17" s="124"/>
+      <c r="B17" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="94" t="s">
+      <c r="C17" s="93" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="9" t="s">
@@ -2971,8 +3009,8 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="125"/>
-      <c r="B18" s="95" t="s">
+      <c r="A18" s="124"/>
+      <c r="B18" s="94" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="28" t="s">
@@ -3010,8 +3048,8 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="125"/>
-      <c r="B19" s="95" t="s">
+      <c r="A19" s="124"/>
+      <c r="B19" s="94" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="28" t="s">
@@ -3049,8 +3087,8 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="125"/>
-      <c r="B20" s="95" t="s">
+      <c r="A20" s="124"/>
+      <c r="B20" s="94" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="34" t="s">
@@ -3088,8 +3126,8 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="125"/>
-      <c r="B21" s="96" t="s">
+      <c r="A21" s="124"/>
+      <c r="B21" s="95" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="28" t="s">
@@ -3122,8 +3160,8 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="125"/>
-      <c r="B22" s="96" t="s">
+      <c r="A22" s="124"/>
+      <c r="B22" s="95" t="s">
         <v>15</v>
       </c>
       <c r="C22" s="28" t="s">
@@ -3161,8 +3199,8 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="125"/>
-      <c r="B23" s="96" t="s">
+      <c r="A23" s="124"/>
+      <c r="B23" s="95" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="28" t="s">
@@ -3200,8 +3238,8 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="125"/>
-      <c r="B24" s="96" t="s">
+      <c r="A24" s="124"/>
+      <c r="B24" s="95" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="28" t="s">
@@ -3239,8 +3277,8 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="125"/>
-      <c r="B25" s="96" t="s">
+      <c r="A25" s="124"/>
+      <c r="B25" s="95" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="28" t="s">
@@ -3278,35 +3316,35 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="125"/>
-      <c r="B26" s="97" t="s">
+      <c r="A26" s="124"/>
+      <c r="B26" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="92" t="s">
+      <c r="C26" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="84" t="s">
+      <c r="D26" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="84"/>
-      <c r="F26" s="84">
+      <c r="E26" s="83"/>
+      <c r="F26" s="83">
         <v>20.57</v>
       </c>
-      <c r="G26" s="84">
+      <c r="G26" s="83">
         <f t="shared" si="1"/>
         <v>24.684000000000001</v>
       </c>
-      <c r="H26" s="85">
+      <c r="H26" s="84">
         <v>0.1</v>
       </c>
-      <c r="I26" s="84">
+      <c r="I26" s="83">
         <v>2</v>
       </c>
-      <c r="J26" s="86">
+      <c r="J26" s="85">
         <f t="shared" si="2"/>
         <v>37.026000000000003</v>
       </c>
-      <c r="K26" s="87">
+      <c r="K26" s="86">
         <f t="shared" si="3"/>
         <v>44.431200000000004</v>
       </c>
@@ -3315,7 +3353,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="125"/>
+      <c r="A27" s="134"/>
       <c r="B27" s="77" t="s">
         <v>83</v>
       </c>
@@ -3349,7 +3387,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="125"/>
+      <c r="A28" s="134"/>
       <c r="B28" s="80" t="s">
         <v>83</v>
       </c>
@@ -3386,7 +3424,7 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="125"/>
+      <c r="A29" s="134"/>
       <c r="B29" s="80" t="s">
         <v>83</v>
       </c>
@@ -3423,7 +3461,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="125"/>
+      <c r="A30" s="134"/>
       <c r="B30" s="80" t="s">
         <v>83</v>
       </c>
@@ -3459,7 +3497,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="125"/>
+      <c r="A31" s="134"/>
       <c r="B31" s="80" t="s">
         <v>83</v>
       </c>
@@ -3493,7 +3531,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="125"/>
+      <c r="A32" s="134"/>
       <c r="B32" s="80" t="s">
         <v>83</v>
       </c>
@@ -3530,7 +3568,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="125"/>
+      <c r="A33" s="134"/>
       <c r="B33" s="80" t="s">
         <v>83</v>
       </c>
@@ -3567,7 +3605,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="125"/>
+      <c r="A34" s="134"/>
       <c r="B34" s="80" t="s">
         <v>83</v>
       </c>
@@ -3604,7 +3642,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="125"/>
+      <c r="A35" s="134"/>
       <c r="B35" s="80" t="s">
         <v>83</v>
       </c>
@@ -3643,7 +3681,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="125"/>
+      <c r="A36" s="134"/>
       <c r="B36" s="80" t="s">
         <v>83</v>
       </c>
@@ -3679,7 +3717,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="125"/>
+      <c r="A37" s="134"/>
       <c r="B37" s="80" t="s">
         <v>83</v>
       </c>
@@ -3716,7 +3754,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="125"/>
+      <c r="A38" s="134"/>
       <c r="B38" s="80" t="s">
         <v>83</v>
       </c>
@@ -3753,7 +3791,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="125"/>
+      <c r="A39" s="134"/>
       <c r="B39" s="80" t="s">
         <v>83</v>
       </c>
@@ -3790,7 +3828,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="125"/>
+      <c r="A40" s="134"/>
       <c r="B40" s="80" t="s">
         <v>83</v>
       </c>
@@ -3805,7 +3843,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="G40" s="29">
-        <f t="shared" ref="G40:G47" si="9">1.2*F40</f>
+        <f t="shared" ref="G40:G49" si="9">1.2*F40</f>
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="H40" s="36">
@@ -3815,11 +3853,11 @@
         <v>50</v>
       </c>
       <c r="J40" s="31">
-        <f t="shared" ref="J40:J47" si="10">I40*F40*(1-H40)</f>
+        <f t="shared" ref="J40:J49" si="10">I40*F40*(1-H40)</f>
         <v>1.5750000000000002</v>
       </c>
       <c r="K40" s="81">
-        <f t="shared" ref="K40:K47" si="11">J40*1.2</f>
+        <f t="shared" ref="K40:K49" si="11">J40*1.2</f>
         <v>1.8900000000000001</v>
       </c>
       <c r="L40" t="s">
@@ -3827,7 +3865,7 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="125"/>
+      <c r="A41" s="134"/>
       <c r="B41" s="80" t="s">
         <v>83</v>
       </c>
@@ -3842,7 +3880,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="G41" s="29">
-        <f t="shared" ref="G41:G44" si="12">1.2*F41</f>
+        <f t="shared" ref="G41:G46" si="12">1.2*F41</f>
         <v>4.4399999999999995E-2</v>
       </c>
       <c r="H41" s="36">
@@ -3864,7 +3902,7 @@
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="125"/>
+      <c r="A42" s="134"/>
       <c r="B42" s="80" t="s">
         <v>83</v>
       </c>
@@ -3900,36 +3938,36 @@
         <v>232</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="125"/>
-      <c r="B43" s="82" t="s">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="134"/>
+      <c r="B43" s="130" t="s">
         <v>83</v>
       </c>
-      <c r="C43" s="83" t="s">
+      <c r="C43" s="135" t="s">
         <v>243</v>
       </c>
-      <c r="D43" s="84" t="s">
+      <c r="D43" s="14" t="s">
         <v>244</v>
       </c>
-      <c r="E43" s="84"/>
-      <c r="F43" s="84">
+      <c r="E43" s="14"/>
+      <c r="F43" s="14">
         <v>0.25800000000000001</v>
       </c>
-      <c r="G43" s="84">
+      <c r="G43" s="14">
         <f t="shared" si="12"/>
         <v>0.30959999999999999</v>
       </c>
-      <c r="H43" s="85">
+      <c r="H43" s="15">
         <v>0.1</v>
       </c>
-      <c r="I43" s="84">
+      <c r="I43" s="14">
         <v>25</v>
       </c>
-      <c r="J43" s="86">
+      <c r="J43" s="16">
         <f t="shared" si="13"/>
         <v>5.8050000000000006</v>
       </c>
-      <c r="K43" s="87">
+      <c r="K43" s="17">
         <f t="shared" si="14"/>
         <v>6.9660000000000002</v>
       </c>
@@ -3938,600 +3976,649 @@
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="125"/>
-      <c r="B44" s="111" t="s">
+      <c r="A44" s="134"/>
+      <c r="B44" s="136" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="135"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="17"/>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="134"/>
+      <c r="B45" s="137" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="82" t="s">
+        <v>256</v>
+      </c>
+      <c r="D45" s="83" t="s">
+        <v>253</v>
+      </c>
+      <c r="E45" s="83"/>
+      <c r="F45" s="83">
+        <v>13.88</v>
+      </c>
+      <c r="G45" s="83">
+        <f t="shared" ref="G45" si="15">1.2*F45</f>
+        <v>16.655999999999999</v>
+      </c>
+      <c r="H45" s="84">
+        <v>0.1</v>
+      </c>
+      <c r="I45" s="83">
+        <v>1</v>
+      </c>
+      <c r="J45" s="85">
+        <f t="shared" ref="J45" si="16">I45*F45*(1-H45)</f>
+        <v>12.492000000000001</v>
+      </c>
+      <c r="K45" s="86">
+        <f t="shared" ref="K45" si="17">J45*1.2</f>
+        <v>14.990400000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="124"/>
+      <c r="B46" s="110" t="s">
         <v>197</v>
       </c>
-      <c r="C44" s="109" t="s">
+      <c r="C46" s="108" t="s">
         <v>252</v>
       </c>
-      <c r="D44" s="110" t="s">
+      <c r="D46" s="109" t="s">
         <v>253</v>
       </c>
-      <c r="E44" s="110"/>
-      <c r="F44" s="110">
+      <c r="E46" s="109"/>
+      <c r="F46" s="109">
         <v>16.28</v>
       </c>
-      <c r="G44" s="14">
+      <c r="G46" s="109">
         <f t="shared" si="12"/>
         <v>19.536000000000001</v>
       </c>
-      <c r="H44" s="15">
+      <c r="H46" s="131">
         <v>0.1</v>
       </c>
-      <c r="I44" s="110">
+      <c r="I46" s="109">
         <v>1</v>
       </c>
-      <c r="J44" s="16">
-        <f t="shared" ref="J44" si="15">I44*F44*(1-H44)</f>
+      <c r="J46" s="132">
+        <f t="shared" ref="J46" si="18">I46*F46*(1-H46)</f>
         <v>14.652000000000001</v>
       </c>
-      <c r="K44" s="17">
-        <f t="shared" ref="K44" si="16">J44*1.2</f>
+      <c r="K46" s="133">
+        <f t="shared" ref="K46" si="19">J46*1.2</f>
         <v>17.5824</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="125"/>
-      <c r="B45" s="112" t="s">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="124"/>
+      <c r="B47" s="111" t="s">
         <v>197</v>
       </c>
-      <c r="C45" s="28" t="s">
+      <c r="C47" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="D45" s="29" t="s">
+      <c r="D47" s="29" t="s">
         <v>215</v>
       </c>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29">
+      <c r="E47" s="29"/>
+      <c r="F47" s="29">
         <v>0.45200000000000001</v>
       </c>
-      <c r="G45" s="29">
+      <c r="G47" s="29">
         <f t="shared" si="9"/>
         <v>0.54239999999999999</v>
       </c>
-      <c r="H45" s="36">
+      <c r="H47" s="36">
         <v>0.1</v>
       </c>
-      <c r="I45" s="29">
+      <c r="I47" s="29">
         <v>5</v>
       </c>
-      <c r="J45" s="31">
+      <c r="J47" s="31">
         <f t="shared" si="10"/>
         <v>2.0340000000000003</v>
       </c>
-      <c r="K45" s="81">
+      <c r="K47" s="81">
         <f t="shared" si="11"/>
         <v>2.4408000000000003</v>
       </c>
-      <c r="L45" t="s">
+      <c r="L47" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="125"/>
-      <c r="B46" s="88" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="124"/>
+      <c r="B48" s="87" t="s">
         <v>197</v>
       </c>
-      <c r="C46" s="28" t="s">
+      <c r="C48" s="28" t="s">
         <v>216</v>
       </c>
-      <c r="D46" s="29" t="s">
+      <c r="D48" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="E46" s="29" t="s">
+      <c r="E48" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F46" s="29">
+      <c r="F48" s="29">
         <v>0.105</v>
       </c>
-      <c r="G46" s="29">
+      <c r="G48" s="29">
         <f t="shared" si="9"/>
         <v>0.126</v>
       </c>
-      <c r="H46" s="36">
+      <c r="H48" s="36">
         <v>0.1</v>
       </c>
-      <c r="I46" s="29">
+      <c r="I48" s="29">
         <v>10</v>
       </c>
-      <c r="J46" s="31">
+      <c r="J48" s="31">
         <f t="shared" si="10"/>
         <v>0.94500000000000006</v>
       </c>
-      <c r="K46" s="81">
+      <c r="K48" s="81">
         <f t="shared" si="11"/>
         <v>1.1340000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="125"/>
-      <c r="B47" s="88" t="s">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="124"/>
+      <c r="B49" s="87" t="s">
         <v>197</v>
       </c>
-      <c r="C47" s="28" t="s">
+      <c r="C49" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="D47" s="29" t="s">
+      <c r="D49" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="E47" s="29" t="s">
+      <c r="E49" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="F47" s="29">
+      <c r="F49" s="29">
         <v>0.51</v>
       </c>
-      <c r="G47" s="29">
+      <c r="G49" s="29">
         <f t="shared" si="9"/>
         <v>0.61199999999999999</v>
       </c>
-      <c r="H47" s="36">
+      <c r="H49" s="36">
         <v>0.1</v>
       </c>
-      <c r="I47" s="29">
+      <c r="I49" s="29">
         <v>10</v>
       </c>
-      <c r="J47" s="31">
+      <c r="J49" s="31">
         <f t="shared" si="10"/>
         <v>4.59</v>
       </c>
-      <c r="K47" s="81">
+      <c r="K49" s="81">
         <f t="shared" si="11"/>
         <v>5.508</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="125"/>
-      <c r="B48" s="88" t="s">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="124"/>
+      <c r="B50" s="87" t="s">
         <v>197</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C50" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="D48" s="29" t="s">
+      <c r="D50" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="E48" s="29" t="s">
+      <c r="E50" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F48" s="29">
+      <c r="F50" s="29">
         <v>2.54</v>
       </c>
-      <c r="G48" s="29">
+      <c r="G50" s="29">
         <f t="shared" si="1"/>
         <v>3.048</v>
       </c>
-      <c r="H48" s="36">
+      <c r="H50" s="36">
         <v>0.1</v>
       </c>
-      <c r="I48" s="29">
+      <c r="I50" s="29">
         <v>1</v>
       </c>
-      <c r="J48" s="31">
+      <c r="J50" s="31">
         <f t="shared" si="2"/>
         <v>2.286</v>
       </c>
-      <c r="K48" s="81">
+      <c r="K50" s="81">
         <f t="shared" si="3"/>
         <v>2.7431999999999999</v>
       </c>
-      <c r="L48" t="s">
+      <c r="L50" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="125"/>
-      <c r="B49" s="91" t="s">
+    <row r="51" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="124"/>
+      <c r="B51" s="90" t="s">
         <v>197</v>
       </c>
-      <c r="C49" s="92" t="s">
+      <c r="C51" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="D49" s="84" t="s">
+      <c r="D51" s="83" t="s">
         <v>225</v>
       </c>
-      <c r="E49" s="84" t="s">
+      <c r="E51" s="83" t="s">
         <v>65</v>
       </c>
-      <c r="F49" s="84">
+      <c r="F51" s="83">
         <v>1.76</v>
       </c>
-      <c r="G49" s="84">
-        <f t="shared" ref="G49" si="17">1.2*F49</f>
+      <c r="G51" s="83">
+        <f t="shared" ref="G51" si="20">1.2*F51</f>
         <v>2.1120000000000001</v>
       </c>
-      <c r="H49" s="85">
+      <c r="H51" s="84">
         <v>0.1</v>
       </c>
-      <c r="I49" s="84">
+      <c r="I51" s="83">
         <v>10</v>
       </c>
-      <c r="J49" s="86">
-        <f t="shared" ref="J49" si="18">I49*F49*(1-H49)</f>
+      <c r="J51" s="85">
+        <f t="shared" ref="J51" si="21">I51*F51*(1-H51)</f>
         <v>15.840000000000002</v>
       </c>
-      <c r="K49" s="87">
-        <f t="shared" ref="K49" si="19">J49*1.2</f>
+      <c r="K51" s="86">
+        <f t="shared" ref="K51" si="22">J51*1.2</f>
         <v>19.008000000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="125"/>
-      <c r="B50" s="104" t="s">
+    <row r="52" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="124"/>
+      <c r="B52" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="C50" s="94" t="s">
+      <c r="C52" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D52" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E52" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F50" s="9">
+      <c r="F52" s="9">
         <v>30.97</v>
       </c>
-      <c r="G50" s="9">
-        <f>1.2*F50</f>
+      <c r="G52" s="9">
+        <f>1.2*F52</f>
         <v>37.163999999999994</v>
       </c>
-      <c r="H50" s="10">
+      <c r="H52" s="10">
         <v>0.1</v>
       </c>
-      <c r="I50" s="9">
+      <c r="I52" s="9">
         <v>2</v>
       </c>
-      <c r="J50" s="11">
-        <f>I50*F50*(1-H50)</f>
+      <c r="J52" s="11">
+        <f>I52*F52*(1-H52)</f>
         <v>55.746000000000002</v>
       </c>
-      <c r="K50" s="12">
-        <f>J50*1.2</f>
+      <c r="K52" s="12">
+        <f>J52*1.2</f>
         <v>66.895200000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="125"/>
-      <c r="B51" s="105" t="s">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="124"/>
+      <c r="B53" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="C51" s="28" t="s">
+      <c r="C53" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D51" s="29" t="s">
+      <c r="D53" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E51" s="29" t="s">
+      <c r="E53" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="F51" s="29">
+      <c r="F53" s="29">
         <v>16</v>
       </c>
-      <c r="G51" s="29">
-        <f>1.2*F51</f>
+      <c r="G53" s="29">
+        <f>1.2*F53</f>
         <v>19.2</v>
-      </c>
-      <c r="H51" s="36">
-        <v>0.1</v>
-      </c>
-      <c r="I51" s="29">
-        <v>1</v>
-      </c>
-      <c r="J51" s="31">
-        <f>I51*F51*(1-H51)</f>
-        <v>14.4</v>
-      </c>
-      <c r="K51" s="81">
-        <f>J51*1.2</f>
-        <v>17.28</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="125"/>
-      <c r="B52" s="105" t="s">
-        <v>24</v>
-      </c>
-      <c r="C52" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D52" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="E52" s="106" t="s">
-        <v>32</v>
-      </c>
-      <c r="F52" s="29">
-        <v>16.47</v>
-      </c>
-      <c r="G52" s="29">
-        <f>1.2*F52</f>
-        <v>19.763999999999999</v>
-      </c>
-      <c r="H52" s="36">
-        <v>0.1</v>
-      </c>
-      <c r="I52" s="29">
-        <v>1</v>
-      </c>
-      <c r="J52" s="31">
-        <f>I52*F52*(1-H52)</f>
-        <v>14.822999999999999</v>
-      </c>
-      <c r="K52" s="81">
-        <f>J52*1.2</f>
-        <v>17.787599999999998</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="125"/>
-      <c r="B53" s="105" t="s">
-        <v>24</v>
-      </c>
-      <c r="C53" s="120" t="s">
-        <v>103</v>
-      </c>
-      <c r="D53" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="E53" s="29"/>
-      <c r="F53" s="38">
-        <v>1.45</v>
-      </c>
-      <c r="G53" s="29">
-        <f t="shared" si="1"/>
-        <v>1.74</v>
       </c>
       <c r="H53" s="36">
         <v>0.1</v>
       </c>
-      <c r="I53" s="33">
+      <c r="I53" s="29">
         <v>1</v>
       </c>
       <c r="J53" s="31">
+        <f>I53*F53*(1-H53)</f>
+        <v>14.4</v>
+      </c>
+      <c r="K53" s="81">
+        <f>J53*1.2</f>
+        <v>17.28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="124"/>
+      <c r="B54" s="104" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D54" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54" s="105" t="s">
+        <v>32</v>
+      </c>
+      <c r="F54" s="29">
+        <v>16.47</v>
+      </c>
+      <c r="G54" s="29">
+        <f>1.2*F54</f>
+        <v>19.763999999999999</v>
+      </c>
+      <c r="H54" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="I54" s="29">
+        <v>1</v>
+      </c>
+      <c r="J54" s="31">
+        <f>I54*F54*(1-H54)</f>
+        <v>14.822999999999999</v>
+      </c>
+      <c r="K54" s="81">
+        <f>J54*1.2</f>
+        <v>17.787599999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="124"/>
+      <c r="B55" s="104" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="119" t="s">
+        <v>103</v>
+      </c>
+      <c r="D55" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="E55" s="29"/>
+      <c r="F55" s="38">
+        <v>1.45</v>
+      </c>
+      <c r="G55" s="29">
+        <f t="shared" si="1"/>
+        <v>1.74</v>
+      </c>
+      <c r="H55" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="I55" s="33">
+        <v>1</v>
+      </c>
+      <c r="J55" s="31">
         <f t="shared" si="2"/>
         <v>1.3049999999999999</v>
       </c>
-      <c r="K53" s="81">
+      <c r="K55" s="81">
         <f t="shared" si="3"/>
         <v>1.5659999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="125"/>
-      <c r="B54" s="105" t="s">
+    <row r="56" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="124"/>
+      <c r="B56" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="121" t="s">
+      <c r="C56" s="120" t="s">
         <v>105</v>
       </c>
-      <c r="D54" s="33" t="s">
+      <c r="D56" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="E54" s="29"/>
-      <c r="F54" s="38">
+      <c r="E56" s="29"/>
+      <c r="F56" s="38">
         <v>1.9</v>
       </c>
-      <c r="G54" s="29">
+      <c r="G56" s="29">
         <f t="shared" si="1"/>
         <v>2.2799999999999998</v>
       </c>
-      <c r="H54" s="36">
+      <c r="H56" s="36">
         <v>0.1</v>
       </c>
-      <c r="I54" s="33">
+      <c r="I56" s="33">
         <v>1</v>
       </c>
-      <c r="J54" s="31">
+      <c r="J56" s="31">
         <f t="shared" si="2"/>
         <v>1.71</v>
       </c>
-      <c r="K54" s="81">
+      <c r="K56" s="81">
         <f t="shared" si="3"/>
         <v>2.052</v>
       </c>
-      <c r="L54" s="39" t="s">
+      <c r="L56" s="39" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="125"/>
-      <c r="B55" s="105" t="s">
+    <row r="57" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="124"/>
+      <c r="B57" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="C55" s="121" t="s">
+      <c r="C57" s="120" t="s">
         <v>108</v>
       </c>
-      <c r="D55" s="33" t="s">
+      <c r="D57" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="E55" s="29"/>
-      <c r="F55" s="38">
+      <c r="E57" s="29"/>
+      <c r="F57" s="38">
         <v>0.36</v>
       </c>
-      <c r="G55" s="29">
+      <c r="G57" s="29">
         <f t="shared" si="1"/>
         <v>0.432</v>
       </c>
-      <c r="H55" s="36">
+      <c r="H57" s="36">
         <v>0.1</v>
       </c>
-      <c r="I55" s="33">
+      <c r="I57" s="33">
         <v>10</v>
       </c>
-      <c r="J55" s="31">
+      <c r="J57" s="31">
         <f t="shared" si="2"/>
         <v>3.2399999999999998</v>
       </c>
-      <c r="K55" s="81">
+      <c r="K57" s="81">
         <f t="shared" si="3"/>
         <v>3.8879999999999995</v>
       </c>
-      <c r="L55" s="39" t="s">
+      <c r="L57" s="39" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="125"/>
-      <c r="B56" s="105" t="s">
+    <row r="58" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="124"/>
+      <c r="B58" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="121" t="s">
+      <c r="C58" s="120" t="s">
         <v>110</v>
       </c>
-      <c r="D56" s="33" t="s">
+      <c r="D58" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="E56" s="29"/>
-      <c r="F56" s="38">
+      <c r="E58" s="29"/>
+      <c r="F58" s="38">
         <v>0.19</v>
       </c>
-      <c r="G56" s="29">
+      <c r="G58" s="29">
         <f t="shared" si="1"/>
         <v>0.22799999999999998</v>
       </c>
-      <c r="H56" s="36">
+      <c r="H58" s="36">
         <v>0.1</v>
       </c>
-      <c r="I56" s="33">
+      <c r="I58" s="33">
         <v>25</v>
       </c>
-      <c r="J56" s="31">
+      <c r="J58" s="31">
         <f t="shared" si="2"/>
         <v>4.2750000000000004</v>
       </c>
-      <c r="K56" s="81">
+      <c r="K58" s="81">
         <f t="shared" si="3"/>
         <v>5.13</v>
       </c>
-      <c r="L56" s="39" t="s">
+      <c r="L58" s="39" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="125"/>
-      <c r="B57" s="105" t="s">
+    <row r="59" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="124"/>
+      <c r="B59" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="121" t="s">
+      <c r="C59" s="120" t="s">
         <v>112</v>
       </c>
-      <c r="D57" s="33" t="s">
+      <c r="D59" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="E57" s="29"/>
-      <c r="F57" s="38">
+      <c r="E59" s="29"/>
+      <c r="F59" s="38">
         <v>0.11</v>
       </c>
-      <c r="G57" s="29">
+      <c r="G59" s="29">
         <f t="shared" si="1"/>
         <v>0.13200000000000001</v>
       </c>
-      <c r="H57" s="36">
+      <c r="H59" s="36">
         <v>0.1</v>
       </c>
-      <c r="I57" s="33">
+      <c r="I59" s="33">
         <v>25</v>
       </c>
-      <c r="J57" s="31">
+      <c r="J59" s="31">
         <f t="shared" si="2"/>
         <v>2.4750000000000001</v>
       </c>
-      <c r="K57" s="81">
+      <c r="K59" s="81">
         <f t="shared" si="3"/>
         <v>2.97</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="125"/>
-      <c r="B58" s="105" t="s">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="124"/>
+      <c r="B60" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="121" t="s">
+      <c r="C60" s="120" t="s">
         <v>114</v>
       </c>
-      <c r="D58" s="33" t="s">
+      <c r="D60" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="E58" s="29"/>
-      <c r="F58" s="38">
+      <c r="E60" s="29"/>
+      <c r="F60" s="38">
         <v>0.67200000000000004</v>
       </c>
-      <c r="G58" s="29">
+      <c r="G60" s="29">
         <f t="shared" si="1"/>
         <v>0.80640000000000001</v>
       </c>
-      <c r="H58" s="36">
+      <c r="H60" s="36">
         <v>0.1</v>
       </c>
-      <c r="I58" s="33">
+      <c r="I60" s="33">
         <v>5</v>
       </c>
-      <c r="J58" s="31">
+      <c r="J60" s="31">
         <f t="shared" si="2"/>
         <v>3.0240000000000005</v>
       </c>
-      <c r="K58" s="81">
+      <c r="K60" s="81">
         <f t="shared" si="3"/>
         <v>3.6288000000000005</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="126"/>
-      <c r="B59" s="89" t="s">
+    <row r="61" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="125"/>
+      <c r="B61" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="122" t="s">
+      <c r="C61" s="121" t="s">
         <v>116</v>
       </c>
-      <c r="D59" s="90" t="s">
+      <c r="D61" s="89" t="s">
         <v>224</v>
       </c>
-      <c r="E59" s="84"/>
-      <c r="F59" s="84">
+      <c r="E61" s="83"/>
+      <c r="F61" s="83">
         <v>0.156</v>
       </c>
-      <c r="G59" s="84">
+      <c r="G61" s="83">
         <f t="shared" si="1"/>
         <v>0.18720000000000001</v>
       </c>
-      <c r="H59" s="85">
+      <c r="H61" s="84">
         <v>0.1</v>
       </c>
-      <c r="I59" s="84">
+      <c r="I61" s="83">
         <v>50</v>
       </c>
-      <c r="J59" s="86">
+      <c r="J61" s="85">
         <f t="shared" si="2"/>
         <v>7.02</v>
       </c>
-      <c r="K59" s="87">
+      <c r="K61" s="86">
         <f t="shared" si="3"/>
         <v>8.4239999999999995</v>
       </c>
-      <c r="L59" s="39" t="s">
+      <c r="L61" s="39" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E60" s="113" t="s">
+    <row r="62" spans="1:12" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E62" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="F60" s="114"/>
-      <c r="G60" s="114"/>
-      <c r="H60" s="114"/>
-      <c r="I60" s="114"/>
-      <c r="J60" s="114"/>
-      <c r="K60" s="115">
-        <f>SUM(K7:K59)</f>
-        <v>647.87364000000002</v>
+      <c r="F62" s="113"/>
+      <c r="G62" s="113"/>
+      <c r="H62" s="113"/>
+      <c r="I62" s="113"/>
+      <c r="J62" s="113"/>
+      <c r="K62" s="114">
+        <f>SUM(K7:K61)</f>
+        <v>662.86404000000005</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A59"/>
+    <mergeCell ref="A7:A61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4554,7 +4641,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B10:B15 B17:B26 B35:B59 B7:B8</xm:sqref>
+          <xm:sqref>B10:B15 B17:B26 B35:B61 B7:B8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -6596,14 +6683,14 @@
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="45"/>
-      <c r="E17" s="127" t="s">
+      <c r="E17" s="126" t="s">
         <v>220</v>
       </c>
-      <c r="F17" s="127"/>
-      <c r="G17" s="127"/>
-      <c r="H17" s="127"/>
-      <c r="I17" s="127"/>
-      <c r="J17" s="128">
+      <c r="F17" s="126"/>
+      <c r="G17" s="126"/>
+      <c r="H17" s="126"/>
+      <c r="I17" s="126"/>
+      <c r="J17" s="127">
         <f>SUM(J2:J15)</f>
         <v>101.52000000000001</v>
       </c>
@@ -6611,12 +6698,12 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="45"/>
-      <c r="E18" s="127"/>
-      <c r="F18" s="127"/>
-      <c r="G18" s="127"/>
-      <c r="H18" s="127"/>
-      <c r="I18" s="127"/>
-      <c r="J18" s="128"/>
+      <c r="E18" s="126"/>
+      <c r="F18" s="126"/>
+      <c r="G18" s="126"/>
+      <c r="H18" s="126"/>
+      <c r="I18" s="126"/>
+      <c r="J18" s="127"/>
       <c r="K18" s="47"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -6654,7 +6741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C11" sqref="C11:M11"/>
     </sheetView>
   </sheetViews>
@@ -6735,13 +6822,13 @@
     </row>
     <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="54"/>
-      <c r="E3" s="129" t="s">
+      <c r="E3" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="129"/>
-      <c r="I3" s="129"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
       <c r="J3">
         <f>J2</f>
         <v>305.3</v>
@@ -6794,11 +6881,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="129" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
       <c r="D1" s="55" t="s">
         <v>162</v>
       </c>

</xml_diff>

<commit_message>
Ajout config MK3 Vulcanix v2
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Commandes.xlsx
+++ b/EL - Electrical/Autre/Commandes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\EL - Electrical\Autre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9263E46B-C595-4739-9BD6-69DDEF33D348}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EC8D36-4FAC-4374-B4A8-118E849493E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS components" sheetId="1" r:id="rId1"/>
@@ -5814,7 +5814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -5865,7 +5865,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6172,8 +6172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7339,7 +7339,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Un peu de tout
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Commandes.xlsx
+++ b/EL - Electrical/Autre/Commandes.xlsx
@@ -1,41 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\EL - Electrical\Autre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26757678-4026-4401-82EB-87BD8DA7DA2E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CA91C9-F961-4480-91FC-82CCA11C3AED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS components" sheetId="1" r:id="rId1"/>
     <sheet name="Farnell" sheetId="2" r:id="rId2"/>
-    <sheet name="Mouser" sheetId="4" r:id="rId3"/>
-    <sheet name="Watterott" sheetId="3" r:id="rId4"/>
-    <sheet name="KazTechnologie" sheetId="5" r:id="rId5"/>
-    <sheet name="Texense" sheetId="6" r:id="rId6"/>
-    <sheet name="oscaro" sheetId="7" r:id="rId7"/>
-    <sheet name="Reverchon" sheetId="8" r:id="rId8"/>
-    <sheet name="DTA Fast" sheetId="9" r:id="rId9"/>
-    <sheet name="DUNKERMOTOREN" sheetId="10" r:id="rId10"/>
-    <sheet name="Souriau" sheetId="11" r:id="rId11"/>
-    <sheet name="Racecapture" sheetId="12" r:id="rId12"/>
-    <sheet name="Données" sheetId="13" r:id="rId13"/>
+    <sheet name="Conrad" sheetId="14" r:id="rId3"/>
+    <sheet name="Mouser" sheetId="4" r:id="rId4"/>
+    <sheet name="Watterott" sheetId="3" r:id="rId5"/>
+    <sheet name="KazTechnologie" sheetId="5" r:id="rId6"/>
+    <sheet name="Texense" sheetId="6" r:id="rId7"/>
+    <sheet name="oscaro" sheetId="7" r:id="rId8"/>
+    <sheet name="Reverchon" sheetId="8" r:id="rId9"/>
+    <sheet name="DTA Fast" sheetId="9" r:id="rId10"/>
+    <sheet name="DUNKERMOTOREN" sheetId="10" r:id="rId11"/>
+    <sheet name="Souriau" sheetId="11" r:id="rId12"/>
+    <sheet name="Racecapture" sheetId="12" r:id="rId13"/>
+    <sheet name="Données" sheetId="13" r:id="rId14"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId14"/>
+    <externalReference r:id="rId15"/>
   </externalReferences>
   <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="278">
   <si>
     <t>Système</t>
   </si>
@@ -906,6 +914,21 @@
   <si>
     <t>Offert par RS le sang ( avec 1 mois de retard quand même)</t>
   </si>
+  <si>
+    <t>BV1 -  Prolongateur, Rouge, Série BV, 22 AWG, 16 AWG, 1.25 mm², Vinyl</t>
+  </si>
+  <si>
+    <t>1 paquet de 100</t>
+  </si>
+  <si>
+    <t>cosse pour TDB</t>
+  </si>
+  <si>
+    <t>Cosse femelle superseal</t>
+  </si>
+  <si>
+    <t>Cosse male superseal</t>
+  </si>
 </sst>
 </file>
 
@@ -916,13 +939,20 @@
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-40C];[Red]\-#,##0.00\ [$€-40C]"/>
     <numFmt numFmtId="166" formatCode="#,##0.00&quot; €&quot;;[Red]\-#,##0.00&quot; €&quot;"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -1089,13 +1119,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color rgb="FF454545"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1108,8 +1131,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="25">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1207,12 +1237,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1924,30 +1948,30 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1968,7 +1992,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1991,7 +2015,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2006,19 +2030,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2027,32 +2051,32 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -2067,10 +2091,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2086,7 +2110,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -2124,7 +2148,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2197,15 +2221,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2242,17 +2266,9 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2262,72 +2278,141 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="17" fillId="23" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="22" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="16" fillId="24" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="23" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2733,8 +2818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2802,7 +2887,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="145" t="s">
+      <c r="A2" s="149" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="82" t="s">
@@ -2840,7 +2925,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="145"/>
+      <c r="A3" s="149"/>
       <c r="B3" s="83" t="s">
         <v>15</v>
       </c>
@@ -2874,7 +2959,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="145"/>
+      <c r="A4" s="149"/>
       <c r="B4" s="80"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
@@ -2910,7 +2995,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="145" t="s">
+      <c r="A5" s="149" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="81" t="s">
@@ -2948,7 +3033,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="145"/>
+      <c r="A6" s="149"/>
       <c r="B6" s="80"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -2968,7 +3053,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="155">
+      <c r="A7" s="150">
         <v>3</v>
       </c>
       <c r="B7" s="91" t="s">
@@ -3016,7 +3101,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="156"/>
+      <c r="A8" s="151"/>
       <c r="B8" s="92" t="s">
         <v>11</v>
       </c>
@@ -3062,7 +3147,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="156"/>
+      <c r="A9" s="151"/>
       <c r="B9" s="93" t="s">
         <v>11</v>
       </c>
@@ -3105,7 +3190,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="156"/>
+      <c r="A10" s="151"/>
       <c r="B10" s="94" t="s">
         <v>11</v>
       </c>
@@ -3151,7 +3236,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="156"/>
+      <c r="A11" s="151"/>
       <c r="B11" s="94" t="s">
         <v>11</v>
       </c>
@@ -3197,7 +3282,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="156"/>
+      <c r="A12" s="151"/>
       <c r="B12" s="94" t="s">
         <v>11</v>
       </c>
@@ -3238,7 +3323,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="156"/>
+      <c r="A13" s="151"/>
       <c r="B13" s="94" t="s">
         <v>11</v>
       </c>
@@ -3279,7 +3364,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="156"/>
+      <c r="A14" s="151"/>
       <c r="B14" s="94" t="s">
         <v>11</v>
       </c>
@@ -3320,7 +3405,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="156"/>
+      <c r="A15" s="151"/>
       <c r="B15" s="93" t="s">
         <v>11</v>
       </c>
@@ -3363,7 +3448,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="156"/>
+      <c r="A16" s="151"/>
       <c r="B16" s="95" t="s">
         <v>11</v>
       </c>
@@ -3404,7 +3489,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="156"/>
+      <c r="A17" s="151"/>
       <c r="B17" s="96" t="s">
         <v>15</v>
       </c>
@@ -3447,7 +3532,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="156"/>
+      <c r="A18" s="151"/>
       <c r="B18" s="97" t="s">
         <v>15</v>
       </c>
@@ -3493,7 +3578,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="156"/>
+      <c r="A19" s="151"/>
       <c r="B19" s="97" t="s">
         <v>15</v>
       </c>
@@ -3539,7 +3624,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="156"/>
+      <c r="A20" s="151"/>
       <c r="B20" s="97" t="s">
         <v>15</v>
       </c>
@@ -3585,7 +3670,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="156"/>
+      <c r="A21" s="151"/>
       <c r="B21" s="98" t="s">
         <v>15</v>
       </c>
@@ -3626,7 +3711,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="156"/>
+      <c r="A22" s="151"/>
       <c r="B22" s="98" t="s">
         <v>15</v>
       </c>
@@ -3672,7 +3757,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="156"/>
+      <c r="A23" s="151"/>
       <c r="B23" s="98" t="s">
         <v>15</v>
       </c>
@@ -3718,7 +3803,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="156"/>
+      <c r="A24" s="151"/>
       <c r="B24" s="98" t="s">
         <v>15</v>
       </c>
@@ -3764,7 +3849,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="156"/>
+      <c r="A25" s="151"/>
       <c r="B25" s="98" t="s">
         <v>15</v>
       </c>
@@ -3810,7 +3895,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="156"/>
+      <c r="A26" s="151"/>
       <c r="B26" s="99" t="s">
         <v>15</v>
       </c>
@@ -3854,7 +3939,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="156"/>
+      <c r="A27" s="151"/>
       <c r="B27" s="100" t="s">
         <v>83</v>
       </c>
@@ -3895,7 +3980,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="156"/>
+      <c r="A28" s="151"/>
       <c r="B28" s="101" t="s">
         <v>83</v>
       </c>
@@ -3939,7 +4024,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="156"/>
+      <c r="A29" s="151"/>
       <c r="B29" s="101" t="s">
         <v>83</v>
       </c>
@@ -3983,7 +4068,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="156"/>
+      <c r="A30" s="151"/>
       <c r="B30" s="101" t="s">
         <v>83</v>
       </c>
@@ -4026,7 +4111,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="156"/>
+      <c r="A31" s="151"/>
       <c r="B31" s="101" t="s">
         <v>83</v>
       </c>
@@ -4067,7 +4152,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="156"/>
+      <c r="A32" s="151"/>
       <c r="B32" s="101" t="s">
         <v>83</v>
       </c>
@@ -4111,7 +4196,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="156"/>
+      <c r="A33" s="151"/>
       <c r="B33" s="101" t="s">
         <v>83</v>
       </c>
@@ -4155,7 +4240,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="156"/>
+      <c r="A34" s="151"/>
       <c r="B34" s="101" t="s">
         <v>83</v>
       </c>
@@ -4199,7 +4284,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="156"/>
+      <c r="A35" s="151"/>
       <c r="B35" s="101" t="s">
         <v>83</v>
       </c>
@@ -4245,7 +4330,7 @@
       </c>
     </row>
     <row r="36" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="156"/>
+      <c r="A36" s="151"/>
       <c r="B36" s="101" t="s">
         <v>83</v>
       </c>
@@ -4291,7 +4376,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="156"/>
+      <c r="A37" s="151"/>
       <c r="B37" s="101" t="s">
         <v>83</v>
       </c>
@@ -4335,7 +4420,7 @@
       </c>
     </row>
     <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="156"/>
+      <c r="A38" s="151"/>
       <c r="B38" s="101" t="s">
         <v>83</v>
       </c>
@@ -4379,7 +4464,7 @@
       </c>
     </row>
     <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="156"/>
+      <c r="A39" s="151"/>
       <c r="B39" s="101" t="s">
         <v>83</v>
       </c>
@@ -4423,7 +4508,7 @@
       </c>
     </row>
     <row r="40" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="156"/>
+      <c r="A40" s="151"/>
       <c r="B40" s="101" t="s">
         <v>83</v>
       </c>
@@ -4467,7 +4552,7 @@
       </c>
     </row>
     <row r="41" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="156"/>
+      <c r="A41" s="151"/>
       <c r="B41" s="101" t="s">
         <v>83</v>
       </c>
@@ -4511,7 +4596,7 @@
       </c>
     </row>
     <row r="42" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="156"/>
+      <c r="A42" s="151"/>
       <c r="B42" s="101" t="s">
         <v>83</v>
       </c>
@@ -4555,7 +4640,7 @@
       </c>
     </row>
     <row r="43" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="156"/>
+      <c r="A43" s="151"/>
       <c r="B43" s="102" t="s">
         <v>83</v>
       </c>
@@ -4599,7 +4684,7 @@
       </c>
     </row>
     <row r="44" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="156"/>
+      <c r="A44" s="151"/>
       <c r="B44" s="103" t="s">
         <v>83</v>
       </c>
@@ -4643,7 +4728,7 @@
       </c>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="156"/>
+      <c r="A45" s="151"/>
       <c r="B45" s="104" t="s">
         <v>83</v>
       </c>
@@ -4684,7 +4769,7 @@
       </c>
     </row>
     <row r="46" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="156"/>
+      <c r="A46" s="151"/>
       <c r="B46" s="105" t="s">
         <v>182</v>
       </c>
@@ -4725,7 +4810,7 @@
       </c>
     </row>
     <row r="47" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="156"/>
+      <c r="A47" s="151"/>
       <c r="B47" s="106" t="s">
         <v>182</v>
       </c>
@@ -4769,7 +4854,7 @@
       </c>
     </row>
     <row r="48" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="156"/>
+      <c r="A48" s="151"/>
       <c r="B48" s="107" t="s">
         <v>182</v>
       </c>
@@ -4812,7 +4897,7 @@
       </c>
     </row>
     <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="156"/>
+      <c r="A49" s="151"/>
       <c r="B49" s="107" t="s">
         <v>182</v>
       </c>
@@ -4855,7 +4940,7 @@
       </c>
     </row>
     <row r="50" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="156"/>
+      <c r="A50" s="151"/>
       <c r="B50" s="107" t="s">
         <v>182</v>
       </c>
@@ -4901,7 +4986,7 @@
       </c>
     </row>
     <row r="51" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="156"/>
+      <c r="A51" s="151"/>
       <c r="B51" s="108" t="s">
         <v>182</v>
       </c>
@@ -4945,7 +5030,7 @@
       <c r="P51" s="119"/>
     </row>
     <row r="52" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="156"/>
+      <c r="A52" s="151"/>
       <c r="B52" s="109" t="s">
         <v>24</v>
       </c>
@@ -4988,7 +5073,7 @@
       </c>
     </row>
     <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="156"/>
+      <c r="A53" s="151"/>
       <c r="B53" s="110" t="s">
         <v>24</v>
       </c>
@@ -5031,7 +5116,7 @@
       </c>
     </row>
     <row r="54" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="156"/>
+      <c r="A54" s="151"/>
       <c r="B54" s="110" t="s">
         <v>24</v>
       </c>
@@ -5071,7 +5156,7 @@
       </c>
     </row>
     <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="156"/>
+      <c r="A55" s="151"/>
       <c r="B55" s="110" t="s">
         <v>24</v>
       </c>
@@ -5112,7 +5197,7 @@
       </c>
     </row>
     <row r="56" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="156"/>
+      <c r="A56" s="151"/>
       <c r="B56" s="110" t="s">
         <v>24</v>
       </c>
@@ -5156,7 +5241,7 @@
       </c>
     </row>
     <row r="57" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="156"/>
+      <c r="A57" s="151"/>
       <c r="B57" s="110" t="s">
         <v>24</v>
       </c>
@@ -5200,7 +5285,7 @@
       </c>
     </row>
     <row r="58" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="156"/>
+      <c r="A58" s="151"/>
       <c r="B58" s="110" t="s">
         <v>24</v>
       </c>
@@ -5244,7 +5329,7 @@
       </c>
     </row>
     <row r="59" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="156"/>
+      <c r="A59" s="151"/>
       <c r="B59" s="110" t="s">
         <v>24</v>
       </c>
@@ -5288,7 +5373,7 @@
       </c>
     </row>
     <row r="60" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="156"/>
+      <c r="A60" s="151"/>
       <c r="B60" s="110" t="s">
         <v>24</v>
       </c>
@@ -5332,7 +5417,7 @@
       </c>
     </row>
     <row r="61" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="156"/>
+      <c r="A61" s="151"/>
       <c r="B61" s="110" t="s">
         <v>24</v>
       </c>
@@ -5370,7 +5455,7 @@
       </c>
     </row>
     <row r="62" spans="1:16" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="156"/>
+      <c r="A62" s="151"/>
       <c r="C62" s="86" t="s">
         <v>114</v>
       </c>
@@ -5411,7 +5496,7 @@
       </c>
     </row>
     <row r="63" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="156"/>
+      <c r="A63" s="151"/>
       <c r="B63" s="115" t="s">
         <v>248</v>
       </c>
@@ -5453,17 +5538,17 @@
       </c>
     </row>
     <row r="64" spans="1:16" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="156"/>
+      <c r="A64" s="151"/>
       <c r="C64" s="90"/>
-      <c r="E64" s="159" t="s">
+      <c r="E64" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="F64" s="160"/>
-      <c r="G64" s="160"/>
-      <c r="H64" s="160"/>
-      <c r="I64" s="160"/>
-      <c r="J64" s="160"/>
-      <c r="K64" s="161">
+      <c r="F64" s="142"/>
+      <c r="G64" s="142"/>
+      <c r="H64" s="142"/>
+      <c r="I64" s="142"/>
+      <c r="J64" s="142"/>
+      <c r="K64" s="143">
         <f>SUM(K7:K63)</f>
         <v>679.79412000000002</v>
       </c>
@@ -5472,13 +5557,13 @@
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="158">
+      <c r="A65" s="152">
         <v>4</v>
       </c>
       <c r="B65" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="C65" s="164" t="s">
+      <c r="C65" s="146" t="s">
         <v>267</v>
       </c>
       <c r="D65" s="32" t="s">
@@ -5508,8 +5593,8 @@
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="158"/>
-      <c r="B66" s="165" t="s">
+      <c r="A66" s="152"/>
+      <c r="B66" s="147" t="s">
         <v>182</v>
       </c>
       <c r="C66" s="28" t="s">
@@ -5542,8 +5627,8 @@
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="158"/>
-      <c r="B67" s="166" t="s">
+      <c r="A67" s="152"/>
+      <c r="B67" s="148" t="s">
         <v>11</v>
       </c>
       <c r="C67" s="28" t="s">
@@ -5576,8 +5661,8 @@
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="158"/>
-      <c r="B68" s="165" t="s">
+      <c r="A68" s="152"/>
+      <c r="B68" s="147" t="s">
         <v>182</v>
       </c>
       <c r="C68" s="28" t="s">
@@ -5610,15 +5695,15 @@
       </c>
     </row>
     <row r="69" spans="1:11" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E69" s="157" t="s">
+      <c r="E69" s="140" t="s">
         <v>18</v>
       </c>
-      <c r="F69" s="162"/>
-      <c r="G69" s="162"/>
-      <c r="H69" s="162"/>
-      <c r="I69" s="162"/>
-      <c r="J69" s="162"/>
-      <c r="K69" s="163">
+      <c r="F69" s="144"/>
+      <c r="G69" s="144"/>
+      <c r="H69" s="144"/>
+      <c r="I69" s="144"/>
+      <c r="J69" s="144"/>
+      <c r="K69" s="145">
         <f>SUM(K65:K68)</f>
         <v>23.986799999999999</v>
       </c>
@@ -5669,6 +5754,439 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:J23"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="1025" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F2">
+        <f>1.2*E2</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>H2*E2</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>I2*1.2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3">
+        <f>1.2*E3</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f>H3*E3</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f>I3*1.2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4">
+        <f>1.2*E4</f>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f>H4*E4</f>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f>I4*1.2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="21">
+        <f>SUM(E3:E4)</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="21">
+        <f>SUM(F3:F4)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="21">
+        <f>SUM(G3:G4)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="21">
+        <f>SUM(H3:H4)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="21">
+        <f>SUM(I3:I4)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" ref="F6:F23" si="0">1.2*E6</f>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I23" si="1">H6*E6</f>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J23" si="2">I6*1.2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000000000000}">
+          <x14:formula1>
+            <xm:f>Données!$A$1:$A$3</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>A2:A4 A6:A20</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000001000000}">
+          <x14:formula1>
+            <xm:f>Données!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>A5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
@@ -6130,7 +6648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
@@ -6554,7 +7072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -6709,12 +7227,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6763,8 +7281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6819,13 +7337,13 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="146">
+      <c r="A2" s="153">
         <v>1</v>
       </c>
       <c r="B2" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="175">
         <v>2313118</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -6856,11 +7374,11 @@
       <c r="L2" s="37"/>
     </row>
     <row r="3" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="147"/>
+      <c r="A3" s="154"/>
       <c r="B3" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="128">
+      <c r="C3" s="176">
         <v>488203</v>
       </c>
       <c r="D3" s="128" t="s">
@@ -6888,13 +7406,13 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="148">
+      <c r="A4" s="159">
         <v>2</v>
       </c>
       <c r="B4" s="132" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="175">
         <v>2611923</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -6922,14 +7440,14 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="149"/>
-      <c r="B5" s="142" t="s">
+      <c r="A5" s="160"/>
+      <c r="B5" s="138" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="138">
+      <c r="C5" s="177">
         <v>2576913</v>
       </c>
-      <c r="D5" s="139" t="s">
+      <c r="D5" s="135" t="s">
         <v>260</v>
       </c>
       <c r="E5" s="32"/>
@@ -6955,11 +7473,11 @@
       <c r="L5" s="37"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="149"/>
-      <c r="B6" s="140" t="s">
+      <c r="A6" s="160"/>
+      <c r="B6" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="84">
         <v>2335763</v>
       </c>
       <c r="D6" s="32" t="s">
@@ -6988,11 +7506,11 @@
       <c r="L6" s="37"/>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="149"/>
-      <c r="B7" s="141" t="s">
+      <c r="A7" s="160"/>
+      <c r="B7" s="137" t="s">
         <v>182</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="27">
         <v>1462838</v>
       </c>
       <c r="D7" s="32" t="s">
@@ -7021,11 +7539,11 @@
       <c r="L7" s="37"/>
     </row>
     <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="149"/>
+      <c r="A8" s="160"/>
       <c r="B8" s="133" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="84">
         <v>488203</v>
       </c>
       <c r="D8" s="32" t="s">
@@ -7054,11 +7572,11 @@
       <c r="L8" s="37"/>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="149"/>
+      <c r="A9" s="160"/>
       <c r="B9" s="133" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="84">
         <v>2452544</v>
       </c>
       <c r="D9" s="32" t="s">
@@ -7087,11 +7605,11 @@
       <c r="L9" s="37"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="149"/>
-      <c r="B10" s="135" t="s">
+      <c r="A10" s="160"/>
+      <c r="B10" s="134" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="137">
+      <c r="C10" s="178">
         <v>2822512</v>
       </c>
       <c r="D10" s="128" t="s">
@@ -7120,126 +7638,273 @@
       <c r="L10" s="37"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="150"/>
-      <c r="B11" s="134" t="s">
+      <c r="A11" s="161"/>
+      <c r="B11" s="173" t="s">
         <v>157</v>
       </c>
-      <c r="C11" s="73">
+      <c r="C11" s="176">
         <v>2667832</v>
       </c>
-      <c r="D11" s="143" t="s">
+      <c r="D11" s="174" t="s">
         <v>259</v>
       </c>
-      <c r="E11" s="73"/>
-      <c r="F11" s="125">
+      <c r="E11" s="128"/>
+      <c r="F11" s="129">
         <v>19.670000000000002</v>
       </c>
-      <c r="G11" s="125">
+      <c r="G11" s="129">
         <f t="shared" si="0"/>
         <v>23.604000000000003</v>
       </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="73">
+      <c r="H11" s="14"/>
+      <c r="I11" s="128">
         <v>1</v>
       </c>
-      <c r="J11" s="125">
+      <c r="J11" s="129">
         <f t="shared" si="1"/>
         <v>19.670000000000002</v>
       </c>
-      <c r="K11" s="126">
+      <c r="K11" s="130">
         <f t="shared" si="2"/>
         <v>23.604000000000003</v>
       </c>
       <c r="L11" s="37"/>
     </row>
-    <row r="12" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="63"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="136"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="43"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
+    <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="183">
+        <v>3</v>
+      </c>
+      <c r="B12" s="179" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="175">
+        <v>9972056</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="123">
+        <v>9.09</v>
+      </c>
+      <c r="G12" s="123">
+        <f t="shared" ref="G12:G13" si="3">1.2*F12</f>
+        <v>10.907999999999999</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="8">
+        <v>1</v>
+      </c>
+      <c r="J12" s="123">
+        <f t="shared" ref="J12:J13" si="4">I12*F12</f>
+        <v>9.09</v>
+      </c>
+      <c r="K12" s="124">
+        <f t="shared" ref="K12:K13" si="5">G12*I12</f>
+        <v>10.907999999999999</v>
+      </c>
+      <c r="L12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="184"/>
+      <c r="B13" s="133" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="84">
+        <v>2452544</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="E13" s="32"/>
+      <c r="F13" s="36">
+        <v>0.214</v>
+      </c>
+      <c r="G13" s="36">
+        <f t="shared" si="3"/>
+        <v>0.25679999999999997</v>
+      </c>
+      <c r="H13" s="28"/>
+      <c r="I13" s="32">
+        <v>100</v>
+      </c>
+      <c r="J13" s="36">
+        <f t="shared" si="4"/>
+        <v>21.4</v>
+      </c>
+      <c r="K13" s="131">
+        <f t="shared" si="5"/>
+        <v>25.679999999999996</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="43"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
+      <c r="A14" s="184"/>
+      <c r="B14" s="180" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="84"/>
+      <c r="D14" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36">
+        <f t="shared" ref="G14:G17" si="6">1.2*F14</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="28"/>
+      <c r="I14" s="32">
+        <v>20</v>
+      </c>
+      <c r="J14" s="36">
+        <f t="shared" ref="J14:J17" si="7">I14*F14</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="131">
+        <f t="shared" ref="K14:K17" si="8">G14*I14</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="43"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
+      <c r="A15" s="184"/>
+      <c r="B15" s="180" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="84">
+        <v>2424111</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="36">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="G15" s="36">
+        <f t="shared" si="6"/>
+        <v>8.7599999999999997E-2</v>
+      </c>
+      <c r="H15" s="28"/>
+      <c r="I15" s="32">
+        <v>100</v>
+      </c>
+      <c r="J15" s="36">
+        <f t="shared" si="7"/>
+        <v>7.3</v>
+      </c>
+      <c r="K15" s="131">
+        <f t="shared" si="8"/>
+        <v>8.76</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="43"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="43"/>
-      <c r="C17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="43"/>
+      <c r="A16" s="184"/>
+      <c r="B16" s="133" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="185">
+        <v>1863412</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="E16" s="28"/>
+      <c r="F16" s="36">
+        <v>0.09</v>
+      </c>
+      <c r="G16" s="36">
+        <f t="shared" si="6"/>
+        <v>0.108</v>
+      </c>
+      <c r="H16" s="28"/>
+      <c r="I16" s="32">
+        <v>50</v>
+      </c>
+      <c r="J16" s="36">
+        <f t="shared" si="7"/>
+        <v>4.5</v>
+      </c>
+      <c r="K16" s="131">
+        <f t="shared" si="8"/>
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="184"/>
+      <c r="B17" s="186" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="187">
+        <v>151038</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="125">
+        <v>0.16</v>
+      </c>
+      <c r="G17" s="125">
+        <f t="shared" si="6"/>
+        <v>0.192</v>
+      </c>
+      <c r="H17" s="19"/>
+      <c r="I17" s="73">
+        <v>50</v>
+      </c>
+      <c r="J17" s="125">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="K17" s="126">
+        <f t="shared" si="8"/>
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="182"/>
+      <c r="B18" s="181"/>
+      <c r="C18" s="162"/>
       <c r="I18" s="37"/>
       <c r="J18" s="44"/>
       <c r="K18" s="44"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="43"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F19" s="164" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="164"/>
+      <c r="H19" s="164"/>
+      <c r="I19" s="164"/>
+      <c r="J19" s="164"/>
+      <c r="K19" s="44">
+        <f>SUM(K12:K17)</f>
+        <v>60.347999999999992</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="43"/>
       <c r="I20" s="37"/>
       <c r="J20" s="44"/>
       <c r="K20" s="44"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" s="43"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="F19:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7253,7 +7918,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B2:B3 B12:B22</xm:sqref>
+          <xm:sqref>B2:B3 B14:B15 B18:B22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B907E55F-DD64-43DB-AF65-00BB92578686}">
           <x14:formula1>
@@ -7262,7 +7927,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B11 B4:B10</xm:sqref>
+          <xm:sqref>B4:B13 B16:B17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7271,10 +7936,321 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F248BBE-05E5-4589-8552-F2AB50D90F2A}">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="33.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="121" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="166">
+        <v>1</v>
+      </c>
+      <c r="B2" s="171" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="167">
+        <v>9972056</v>
+      </c>
+      <c r="D2" s="167" t="s">
+        <v>273</v>
+      </c>
+      <c r="E2" s="167"/>
+      <c r="F2" s="168">
+        <v>9.09</v>
+      </c>
+      <c r="G2" s="168">
+        <f t="shared" ref="G2:G7" si="0">1.2*F2</f>
+        <v>10.907999999999999</v>
+      </c>
+      <c r="H2" s="169">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="167">
+        <v>1</v>
+      </c>
+      <c r="J2" s="168">
+        <f t="shared" ref="J2:J7" si="1">I2*F2</f>
+        <v>9.09</v>
+      </c>
+      <c r="K2" s="168">
+        <f t="shared" ref="K2:K7" si="2">G2*I2</f>
+        <v>10.907999999999999</v>
+      </c>
+      <c r="L2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="165"/>
+      <c r="B3" s="172" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="32">
+        <v>2452544</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="E3" s="32"/>
+      <c r="F3" s="36">
+        <v>0.214</v>
+      </c>
+      <c r="G3" s="36">
+        <f t="shared" si="0"/>
+        <v>0.25679999999999997</v>
+      </c>
+      <c r="H3" s="163">
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="32">
+        <v>100</v>
+      </c>
+      <c r="J3" s="36">
+        <f t="shared" si="1"/>
+        <v>21.4</v>
+      </c>
+      <c r="K3" s="36">
+        <f t="shared" si="2"/>
+        <v>25.679999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="165"/>
+      <c r="B4" s="172" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="E4" s="28"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="163">
+        <v>0.1</v>
+      </c>
+      <c r="I4" s="32">
+        <v>101</v>
+      </c>
+      <c r="J4" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K4" s="36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="165"/>
+      <c r="B5" s="172" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="32">
+        <v>2424111</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="36">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="G5" s="36">
+        <f t="shared" si="0"/>
+        <v>8.7599999999999997E-2</v>
+      </c>
+      <c r="H5" s="163">
+        <v>0.1</v>
+      </c>
+      <c r="I5" s="32">
+        <v>102</v>
+      </c>
+      <c r="J5" s="36">
+        <f t="shared" si="1"/>
+        <v>7.4459999999999997</v>
+      </c>
+      <c r="K5" s="36">
+        <f t="shared" si="2"/>
+        <v>8.9352</v>
+      </c>
+      <c r="L5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="165"/>
+      <c r="B6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="28">
+        <v>749730</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="G6" s="28">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+      <c r="H6" s="163">
+        <v>0.1</v>
+      </c>
+      <c r="I6" s="28">
+        <v>50</v>
+      </c>
+      <c r="J6" s="28">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="K6" s="28">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="165"/>
+      <c r="B7" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="170">
+        <v>749706</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28">
+        <v>0.18</v>
+      </c>
+      <c r="G7" s="28">
+        <f t="shared" si="0"/>
+        <v>0.216</v>
+      </c>
+      <c r="H7" s="163">
+        <v>0.1</v>
+      </c>
+      <c r="I7" s="28">
+        <v>50</v>
+      </c>
+      <c r="J7" s="28">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="K7" s="28">
+        <f t="shared" si="2"/>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="165"/>
+      <c r="B8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4FDC7918-19FD-4A20-B78F-E944E8B4F1E0}">
+          <x14:formula1>
+            <xm:f>Données!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>B2:B3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8CB4E303-0A3A-4CC9-BAF7-E52A02AA8F1D}">
+          <x14:formula1>
+            <xm:f>Données!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>B4:B8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
@@ -7754,26 +8730,26 @@
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="43"/>
-      <c r="E16" s="151" t="s">
+      <c r="E16" s="155" t="s">
         <v>205</v>
       </c>
-      <c r="F16" s="151"/>
-      <c r="G16" s="151"/>
-      <c r="H16" s="151"/>
-      <c r="I16" s="151"/>
-      <c r="J16" s="152">
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="156">
         <f>SUM(J2:J14)</f>
         <v>101.52000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="43"/>
-      <c r="E17" s="151"/>
-      <c r="F17" s="151"/>
-      <c r="G17" s="151"/>
-      <c r="H17" s="151"/>
-      <c r="I17" s="151"/>
-      <c r="J17" s="152"/>
+      <c r="E17" s="155"/>
+      <c r="F17" s="155"/>
+      <c r="G17" s="155"/>
+      <c r="H17" s="155"/>
+      <c r="I17" s="155"/>
+      <c r="J17" s="156"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="43"/>
@@ -7806,7 +8782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -7933,7 +8909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -8018,13 +8994,13 @@
     </row>
     <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="50"/>
-      <c r="E3" s="153" t="s">
+      <c r="E3" s="157" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="153"/>
-      <c r="I3" s="153"/>
+      <c r="F3" s="157"/>
+      <c r="G3" s="157"/>
+      <c r="H3" s="157"/>
+      <c r="I3" s="157"/>
       <c r="J3">
         <f>J2</f>
         <v>305.3</v>
@@ -8054,7 +9030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
@@ -8077,12 +9053,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="158" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="154"/>
-      <c r="D1" s="144" t="s">
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="139" t="s">
         <v>156</v>
       </c>
     </row>
@@ -8452,7 +9428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
@@ -8858,7 +9834,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -8927,9 +9903,9 @@
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="e">
         <f>H2*F2</f>
-        <v>15.95</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -8949,9 +9925,9 @@
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="J3">
+      <c r="J3" t="e">
         <f>H3*F3</f>
-        <v>9.9</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -8971,9 +9947,9 @@
       <c r="H4">
         <v>2</v>
       </c>
-      <c r="J4">
+      <c r="J4" t="e">
         <f>H4*F4</f>
-        <v>69.8</v>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -8995,437 +9971,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:J23"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
-    <col min="8" max="1025" width="9.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="42" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D2" t="s">
-        <v>176</v>
-      </c>
-      <c r="F2">
-        <f>1.2*E2</f>
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <f>H2*E2</f>
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <f>I2*1.2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="54" t="s">
-        <v>177</v>
-      </c>
-      <c r="D3" t="s">
-        <v>178</v>
-      </c>
-      <c r="F3">
-        <f>1.2*E3</f>
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <f>H3*E3</f>
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <f>I3*1.2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D4" t="s">
-        <v>180</v>
-      </c>
-      <c r="F4">
-        <f>1.2*E4</f>
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <f>H4*E4</f>
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <f>I4*1.2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="21">
-        <f>SUM(E3:E4)</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="21">
-        <f>SUM(F3:F4)</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="21">
-        <f>SUM(G3:G4)</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="21">
-        <f>SUM(H3:H4)</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="21">
-        <f>SUM(I3:I4)</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F6">
-        <f t="shared" ref="F6:F23" si="0">1.2*E6</f>
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <f t="shared" ref="I6:I23" si="1">H6*E6</f>
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <f t="shared" ref="J6:J23" si="2">I6*1.2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000000000000}">
-          <x14:formula1>
-            <xm:f>Données!$A$1:$A$3</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>A2:A4 A6:A20</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000001000000}">
-          <x14:formula1>
-            <xm:f>Données!$A$1:$A$5</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>A5</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>